<commit_message>
week 2 report: update weekly_report.xlsx
</commit_message>
<xml_diff>
--- a/reports/weekly_report.xlsx
+++ b/reports/weekly_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>ردیف</t>
   </si>
@@ -82,6 +82,22 @@
   </si>
   <si>
     <t>هفته دوم</t>
+  </si>
+  <si>
+    <t>مرور و خواندن مفاهبم پایتون در W3SCHOOL</t>
+  </si>
+  <si>
+    <t>ویدیو های تک قسمتی مونگارد</t>
+  </si>
+  <si>
+    <t>خواندن با تمرکز روی مفاهیم شی گرایی در پایتون</t>
+  </si>
+  <si>
+    <t>کد زدن و تمرین OOP</t>
+  </si>
+  <si>
+    <t>با سمه تعالی
+سلام علیکم، با احترام، جهت استحضار بنده با توجه به اینکه احساس کردم نیاز به فراگیری یک سری مباحث پایه ای دارم این هفته  را با اجازه شما بر روی این مباحث  وقت گذاشتم  و تمرینات self-study  انجام شده در گیت‌هاب قرار گرفت انشاا... از هفته آتی  موارد مورد نظر حضرتعالی را ادامه خواهم داد ضمن این هفته به دلیل باگی که در برنامه پروژه کارشناسی بوجود آماده بود وقت کم تری را روی کار آموزی گذاشتم که در هفته آتی جبران خواهم کرد انشاا..</t>
   </si>
 </sst>
 </file>
@@ -227,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -235,11 +251,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -250,14 +269,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -571,28 +593,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21.6">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="3">
@@ -615,7 +637,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="21.6">
-      <c r="A3" s="6"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="3">
         <f>B2+1</f>
         <v>2</v>
@@ -638,16 +660,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="21.6">
-      <c r="A4" s="6"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="3">
-        <f t="shared" ref="B4:B19" si="0">B3+1</f>
+        <f t="shared" ref="B4:B20" si="0">B3+1</f>
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:D16" si="1">D3+1</f>
+        <f t="shared" ref="D4:D17" si="1">D3+1</f>
         <v>20</v>
       </c>
       <c r="E4" s="3">
@@ -661,7 +683,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="21.6">
-      <c r="A5" s="6"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -684,7 +706,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="129.6">
-      <c r="A6" s="6"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -707,7 +729,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="21.6">
-      <c r="A7" s="6"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -728,7 +750,7 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="108">
-      <c r="A8" s="6"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -751,210 +773,249 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="21.6">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="5">
         <f>SUM(F2:F8)</f>
         <v>22</v>
       </c>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="5" t="s">
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" ht="121.8" customHeight="1">
+      <c r="A10" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <f>B8+1</f>
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="str">
-        <f>C2</f>
+      <c r="C11" s="1" t="str">
+        <f t="shared" ref="C11:C17" si="2">C2</f>
         <v>یکشنبه</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <f>D8+1</f>
         <v>25</v>
       </c>
-      <c r="E10" s="1">
-        <v>8</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="6"/>
-      <c r="B11" s="1">
+      <c r="E11" s="1">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="14"/>
+      <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="1" t="str">
-        <f>C3</f>
+      <c r="C12" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>دوشنبه</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="E11" s="1">
-        <v>8</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="6"/>
-      <c r="B12" s="1">
+      <c r="E12" s="1">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="14"/>
+      <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="1" t="str">
-        <f>C4</f>
+      <c r="C13" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>سه شنبه</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D13" s="1">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="E12" s="1">
-        <v>8</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="6"/>
-      <c r="B13" s="1">
+      <c r="E13" s="1">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="14"/>
+      <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C13" s="1" t="str">
-        <f>C5</f>
+      <c r="C14" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>چهارشنبه</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D14" s="1">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="E13" s="1">
-        <v>8</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="6"/>
-      <c r="B14" s="1">
+      <c r="E14" s="1">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="14"/>
+      <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="str">
-        <f>C6</f>
+      <c r="C15" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>پنج شنبه</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D15" s="1">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="E14" s="1">
-        <v>8</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="6"/>
-      <c r="B15" s="1">
+      <c r="E15" s="1">
+        <v>8</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="14"/>
+      <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="1" t="str">
-        <f>C7</f>
+      <c r="C16" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>جمعه</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D16" s="1">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="E15" s="1">
-        <v>8</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="6"/>
-      <c r="B16" s="1">
+      <c r="E16" s="1">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="14"/>
+      <c r="B17" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16" s="1" t="str">
-        <f>C8</f>
+      <c r="C17" s="1" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">شنبه </v>
       </c>
-      <c r="D16" s="1">
-        <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" ht="21.6">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7" t="s">
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>9</v>
+      </c>
+      <c r="F17" s="1">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="21.6">
+      <c r="A18" s="14"/>
+      <c r="B18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="10">
-        <f>SUM(F10:F16)</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="B18" s="1">
-        <f>B16+1</f>
-        <v>15</v>
-      </c>
-      <c r="C18" s="1" t="str">
-        <f t="shared" ref="C18:C19" si="2">C10</f>
-        <v>یکشنبه</v>
-      </c>
-      <c r="D18" s="1">
-        <f>D16+1</f>
-        <v>32</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="5">
+        <f>SUM(F11:F17)</f>
+        <v>15.5</v>
+      </c>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7">
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f>B17+1</f>
+        <v>15</v>
       </c>
       <c r="C19" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>دوشنبه</v>
-      </c>
-      <c r="D19" s="1"/>
+        <f t="shared" ref="C19:C20" si="3">C11</f>
+        <v>یکشنبه</v>
+      </c>
+      <c r="D19" s="1">
+        <f>D17+1</f>
+        <v>2</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
+    <row r="20" spans="1:7">
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>دوشنبه</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
week 3 report: update weekly_report.xlsx
</commit_message>
<xml_diff>
--- a/reports/weekly_report.xlsx
+++ b/reports/weekly_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>ردیف</t>
   </si>
@@ -98,6 +98,31 @@
   <si>
     <t>با سمه تعالی
 سلام علیکم، با احترام، جهت استحضار بنده با توجه به اینکه احساس کردم نیاز به فراگیری یک سری مباحث پایه ای دارم این هفته  را با اجازه شما بر روی این مباحث  وقت گذاشتم  و تمرینات self-study  انجام شده در گیت‌هاب قرار گرفت انشاا... از هفته آتی  موارد مورد نظر حضرتعالی را ادامه خواهم داد ضمن این هفته به دلیل باگی که در برنامه پروژه کارشناسی بوجود آماده بود وقت کم تری را روی کار آموزی گذاشتم که در هفته آتی جبران خواهم کرد انشاا..</t>
+  </si>
+  <si>
+    <t>on part video and countine self study in sunjects like dunder methods..</t>
+  </si>
+  <si>
+    <t>mongard one part video..</t>
+  </si>
+  <si>
+    <t>contineu on mongard</t>
+  </si>
+  <si>
+    <t>mongard one part video and some coding</t>
+  </si>
+  <si>
+    <t>summerise</t>
+  </si>
+  <si>
+    <t>self-study: about prenciples of oop, decorators , itrators…</t>
+  </si>
+  <si>
+    <t>با سمه تعالی
+سلام علیکم، با احترام، نظر به اینکه روش بنده در دیدن ویدیوها بر اساس ترتیب لیست موجود در سایت نبوده بلکه بر اساس سوالات موجود در ذهن و  نیازی که احساس می کردم بوده و همچنین در کنار تماشای ویدیو ها ،جستجوهائی را برای تکمیل بحث انجام داده و خلاصه نویسی و نکته برداری می کردم لذا علارغم وقت گذاری بیش از 28 ساعت،  از 170 ویدئو تک قسمتی سایت مونگارد تنها موفق به دیدن 60 ویدئو شدم که لیست آن در ابتدای فایل کد پایتون این هفته درج شده است.</t>
+  </si>
+  <si>
+    <t>هفته سوم</t>
   </si>
 </sst>
 </file>
@@ -152,7 +177,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -239,11 +264,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -275,11 +322,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:G10"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -662,7 +717,7 @@
     <row r="4" spans="1:7" ht="21.6">
       <c r="A4" s="14"/>
       <c r="B4" s="3">
-        <f t="shared" ref="B4:B20" si="0">B3+1</f>
+        <f t="shared" ref="B4:B18" si="0">B3+1</f>
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -786,236 +841,416 @@
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="121.8" customHeight="1">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:7" ht="21.6">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="121.8" customHeight="1">
+      <c r="A11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A12" s="16"/>
+      <c r="B12" s="1">
         <f>B8+1</f>
         <v>8</v>
       </c>
-      <c r="C11" s="1" t="str">
-        <f t="shared" ref="C11:C17" si="2">C2</f>
+      <c r="C12" s="1" t="str">
+        <f>C2</f>
         <v>یکشنبه</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
         <f>D8+1</f>
         <v>25</v>
       </c>
-      <c r="E11" s="1">
-        <v>8</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="E12" s="1">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1">
         <v>3.5</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="14"/>
-      <c r="B12" s="1">
+    <row r="13" spans="1:7">
+      <c r="A13" s="16"/>
+      <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C12" s="1" t="str">
+      <c r="C13" s="1" t="str">
+        <f>C3</f>
+        <v>دوشنبه</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="E13" s="1">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="16"/>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>C4</f>
+        <v>سه شنبه</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="E14" s="1">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="16"/>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f>C5</f>
+        <v>چهارشنبه</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="E15" s="1">
+        <v>8</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="16"/>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f>C6</f>
+        <v>پنج شنبه</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="E16" s="1">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="16"/>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f>C7</f>
+        <v>جمعه</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="E17" s="1">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="16"/>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f>C8</f>
+        <v xml:space="preserve">شنبه </v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>9</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="21.6">
+      <c r="A19" s="16"/>
+      <c r="B19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="5">
+        <f>SUM(F12:F18)</f>
+        <v>15.5</v>
+      </c>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:7" ht="21.6">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="152.4" customHeight="1">
+      <c r="A21" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A22" s="16"/>
+      <c r="B22" s="1">
+        <f>B18+1</f>
+        <v>15</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <f t="shared" ref="C22:C23" si="2">C12</f>
+        <v>یکشنبه</v>
+      </c>
+      <c r="D22" s="1">
+        <f>D18+1</f>
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>9</v>
+      </c>
+      <c r="F22" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A23" s="16"/>
+      <c r="B23" s="1">
+        <f>B22+1</f>
+        <v>16</v>
+      </c>
+      <c r="C23" s="1" t="str">
         <f t="shared" si="2"/>
         <v>دوشنبه</v>
       </c>
-      <c r="D12" s="1">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="E12" s="1">
-        <v>8</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="14"/>
-      <c r="B13" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C13" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1">
+        <v>9</v>
+      </c>
+      <c r="F23" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A24" s="16"/>
+      <c r="B24" s="1">
+        <f t="shared" ref="B24:B27" si="3">B23+1</f>
+        <v>17</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <f>C14</f>
         <v>سه شنبه</v>
       </c>
-      <c r="D13" s="1">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="E13" s="1">
-        <v>8</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="14"/>
-      <c r="B14" s="1">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C14" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="D24" s="1">
+        <v>4</v>
+      </c>
+      <c r="E24" s="15">
+        <v>9</v>
+      </c>
+      <c r="F24" s="15">
+        <v>5.5</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A25" s="16"/>
+      <c r="B25" s="1">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f>C15</f>
         <v>چهارشنبه</v>
       </c>
-      <c r="D14" s="1">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="E14" s="1">
-        <v>8</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="14"/>
-      <c r="B15" s="1">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C15" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="D25" s="1">
+        <v>5</v>
+      </c>
+      <c r="E25" s="15">
+        <v>9</v>
+      </c>
+      <c r="F25" s="15">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A26" s="16"/>
+      <c r="B26" s="1">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <f>C16</f>
         <v>پنج شنبه</v>
       </c>
-      <c r="D15" s="1">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="E15" s="1">
-        <v>8</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="14"/>
-      <c r="B16" s="1">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C16" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="D26" s="1">
+        <v>6</v>
+      </c>
+      <c r="E26" s="15">
+        <v>9</v>
+      </c>
+      <c r="F26" s="15">
+        <v>3.75</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A27" s="16"/>
+      <c r="B27" s="1">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f>C17</f>
         <v>جمعه</v>
       </c>
-      <c r="D16" s="1">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="E16" s="1">
-        <v>8</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="14"/>
-      <c r="B17" s="1">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C17" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">شنبه </v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="D27" s="1">
+        <v>7</v>
+      </c>
+      <c r="E27" s="15">
         <v>9</v>
       </c>
-      <c r="F17" s="1">
-        <v>4</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="21.6">
-      <c r="A18" s="14"/>
-      <c r="B18" s="10" t="s">
+      <c r="F27" s="15">
+        <v>2.75</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="19"/>
+      <c r="B28" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="5">
-        <f>SUM(F11:F17)</f>
-        <v>15.5</v>
-      </c>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="B19" s="1">
-        <f>B17+1</f>
-        <v>15</v>
-      </c>
-      <c r="C19" s="1" t="str">
-        <f t="shared" ref="C19:C20" si="3">C11</f>
-        <v>یکشنبه</v>
-      </c>
-      <c r="D19" s="1">
-        <f>D17+1</f>
-        <v>2</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="B20" s="1">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C20" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>دوشنبه</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="19">
+        <f>SUM(F22:F27)</f>
+        <v>26.15</v>
+      </c>
+      <c r="G28" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A21:A27"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="B19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
week 4 report: update weekly_report.xlsx
</commit_message>
<xml_diff>
--- a/reports/weekly_report.xlsx
+++ b/reports/weekly_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
   <si>
     <t>ردیف</t>
   </si>
@@ -123,13 +123,41 @@
   </si>
   <si>
     <t>هفته سوم</t>
+  </si>
+  <si>
+    <t>شنبه</t>
+  </si>
+  <si>
+    <t>هفته چهارم</t>
+  </si>
+  <si>
+    <t>هفته پنجم</t>
+  </si>
+  <si>
+    <t>هفته ششم</t>
+  </si>
+  <si>
+    <t>هفته هفتم</t>
+  </si>
+  <si>
+    <t>mongard one part video</t>
+  </si>
+  <si>
+    <t>contineu on one part video</t>
+  </si>
+  <si>
+    <t>ending mongard one part video and some coding</t>
+  </si>
+  <si>
+    <t>باسمه تعالی
+با سلام احترام، تمام ۱۷۰ ویدیو تک قسمتی سایت مونگارد مشاهده و نکته برداری  و تمرین شد.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,8 +184,15 @@
       <name val="B Nazanin"/>
       <charset val="178"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="B Nazanin"/>
+      <charset val="178"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,8 +211,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -286,11 +327,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -302,40 +378,87 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A27"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -641,37 +764,36 @@
     <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="67.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21.6">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A2" s="13" t="s">
-        <v>19</v>
-      </c>
+      <c r="A2" s="19"/>
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -692,7 +814,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="21.6">
-      <c r="A3" s="14"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="3">
         <f>B2+1</f>
         <v>2</v>
@@ -715,7 +837,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="21.6">
-      <c r="A4" s="14"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B18" si="0">B3+1</f>
         <v>3</v>
@@ -738,7 +860,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="21.6">
-      <c r="A5" s="14"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -761,7 +883,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="129.6">
-      <c r="A6" s="14"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -784,7 +906,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="21.6">
-      <c r="A7" s="14"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -805,7 +927,7 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="108">
-      <c r="A8" s="14"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -828,13 +950,13 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="21.6">
-      <c r="A9" s="14"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="30"/>
+      <c r="B9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="5">
         <f>SUM(F2:F8)</f>
         <v>22</v>
@@ -842,47 +964,47 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="21.6">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="121.8" customHeight="1">
-      <c r="A11" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A12" s="16"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="1">
         <f>B8+1</f>
         <v>8</v>
       </c>
       <c r="C12" s="1" t="str">
-        <f>C2</f>
+        <f t="shared" ref="C12:C17" si="2">C2</f>
         <v>یکشنبه</v>
       </c>
       <c r="D12" s="1">
@@ -900,13 +1022,13 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="16"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C13" s="1" t="str">
-        <f>C3</f>
+        <f t="shared" si="2"/>
         <v>دوشنبه</v>
       </c>
       <c r="D13" s="1">
@@ -924,13 +1046,13 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="16"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C14" s="1" t="str">
-        <f>C4</f>
+        <f t="shared" si="2"/>
         <v>سه شنبه</v>
       </c>
       <c r="D14" s="1">
@@ -948,13 +1070,13 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="16"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C15" s="1" t="str">
-        <f>C5</f>
+        <f t="shared" si="2"/>
         <v>چهارشنبه</v>
       </c>
       <c r="D15" s="1">
@@ -972,13 +1094,13 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="16"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C16" s="1" t="str">
-        <f>C6</f>
+        <f t="shared" si="2"/>
         <v>پنج شنبه</v>
       </c>
       <c r="D16" s="1">
@@ -996,13 +1118,13 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="16"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C17" s="1" t="str">
-        <f>C7</f>
+        <f t="shared" si="2"/>
         <v>جمعه</v>
       </c>
       <c r="D17" s="1">
@@ -1018,7 +1140,7 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="16"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1041,13 +1163,13 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="21.6">
-      <c r="A19" s="16"/>
-      <c r="B19" s="10" t="s">
+      <c r="A19" s="29"/>
+      <c r="B19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="5">
         <f>SUM(F12:F18)</f>
         <v>15.5</v>
@@ -1055,47 +1177,47 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="21.6">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8" t="s">
+      <c r="A20" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="152.4" customHeight="1">
-      <c r="A21" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="18" t="s">
+      <c r="A21" s="14"/>
+      <c r="B21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A22" s="16"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="1">
         <f>B18+1</f>
         <v>15</v>
       </c>
       <c r="C22" s="1" t="str">
-        <f t="shared" ref="C22:C23" si="2">C12</f>
+        <f t="shared" ref="C22:C23" si="3">C12</f>
         <v>یکشنبه</v>
       </c>
       <c r="D22" s="1">
@@ -1113,13 +1235,13 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A23" s="16"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="1">
         <f>B22+1</f>
         <v>16</v>
       </c>
       <c r="C23" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>دوشنبه</v>
       </c>
       <c r="D23" s="1">
@@ -1136,9 +1258,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A24" s="16"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="1">
-        <f t="shared" ref="B24:B27" si="3">B23+1</f>
+        <f t="shared" ref="B24:B27" si="4">B23+1</f>
         <v>17</v>
       </c>
       <c r="C24" s="1" t="str">
@@ -1148,10 +1270,10 @@
       <c r="D24" s="1">
         <v>4</v>
       </c>
-      <c r="E24" s="15">
-        <v>9</v>
-      </c>
-      <c r="F24" s="15">
+      <c r="E24" s="9">
+        <v>9</v>
+      </c>
+      <c r="F24" s="9">
         <v>5.5</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -1159,9 +1281,9 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A25" s="16"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="C25" s="1" t="str">
@@ -1171,10 +1293,10 @@
       <c r="D25" s="1">
         <v>5</v>
       </c>
-      <c r="E25" s="15">
-        <v>9</v>
-      </c>
-      <c r="F25" s="15">
+      <c r="E25" s="9">
+        <v>9</v>
+      </c>
+      <c r="F25" s="9">
         <v>4.4000000000000004</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -1182,9 +1304,9 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A26" s="16"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="C26" s="1" t="str">
@@ -1194,10 +1316,10 @@
       <c r="D26" s="1">
         <v>6</v>
       </c>
-      <c r="E26" s="15">
-        <v>9</v>
-      </c>
-      <c r="F26" s="15">
+      <c r="E26" s="9">
+        <v>9</v>
+      </c>
+      <c r="F26" s="9">
         <v>3.75</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -1205,9 +1327,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A27" s="16"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="C27" s="1" t="str">
@@ -1217,10 +1339,10 @@
       <c r="D27" s="1">
         <v>7</v>
       </c>
-      <c r="E27" s="15">
-        <v>9</v>
-      </c>
-      <c r="F27" s="15">
+      <c r="E27" s="9">
+        <v>9</v>
+      </c>
+      <c r="F27" s="9">
         <v>2.75</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -1228,29 +1350,784 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20" t="s">
+      <c r="A28" s="29"/>
+      <c r="B28" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="19">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="10">
         <f>SUM(F22:F27)</f>
         <v>26.15</v>
       </c>
-      <c r="G28" s="19"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" ht="21.6">
+      <c r="A29" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="40.200000000000003" customHeight="1">
+      <c r="A30" s="14"/>
+      <c r="B30" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="33"/>
+    </row>
+    <row r="31" spans="1:7" ht="21.6">
+      <c r="A31" s="14"/>
+      <c r="B31" s="20">
+        <f>B27+1</f>
+        <v>21</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="20">
+        <f>D27+1</f>
+        <v>8</v>
+      </c>
+      <c r="E31" s="20">
+        <v>9</v>
+      </c>
+      <c r="F31" s="21">
+        <v>2.25</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="21.6">
+      <c r="A32" s="14"/>
+      <c r="B32" s="20">
+        <f>B31+1</f>
+        <v>22</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="20">
+        <f>D31+1</f>
+        <v>9</v>
+      </c>
+      <c r="E32" s="20">
+        <v>9</v>
+      </c>
+      <c r="F32" s="22">
+        <v>3.3</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="21.6">
+      <c r="A33" s="14"/>
+      <c r="B33" s="20">
+        <f t="shared" ref="B33:B37" si="5">B32+1</f>
+        <v>23</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="20">
+        <f t="shared" ref="D33:D37" si="6">D32+1</f>
+        <v>10</v>
+      </c>
+      <c r="E33" s="20">
+        <v>9</v>
+      </c>
+      <c r="F33" s="22">
+        <v>2.85</v>
+      </c>
+      <c r="G33" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="21.6">
+      <c r="A34" s="14"/>
+      <c r="B34" s="20">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="20">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="E34" s="20">
+        <v>9</v>
+      </c>
+      <c r="F34" s="22">
+        <v>2.9</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="21.6">
+      <c r="A35" s="14"/>
+      <c r="B35" s="20">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="20">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="E35" s="20">
+        <v>9</v>
+      </c>
+      <c r="F35" s="22">
+        <v>0</v>
+      </c>
+      <c r="G35" s="22"/>
+    </row>
+    <row r="36" spans="1:7" ht="21.6">
+      <c r="A36" s="14"/>
+      <c r="B36" s="20">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="20">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="E36" s="20">
+        <v>9</v>
+      </c>
+      <c r="F36" s="22">
+        <v>6.6</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="21.6">
+      <c r="A37" s="14"/>
+      <c r="B37" s="20">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="20">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="E37" s="20">
+        <v>9</v>
+      </c>
+      <c r="F37" s="22">
+        <v>1.9</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A38" s="14"/>
+      <c r="B38" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="37">
+        <f>SUM(F31:F37)</f>
+        <v>19.799999999999997</v>
+      </c>
+      <c r="G38" s="37"/>
+    </row>
+    <row r="39" spans="1:7" ht="21.6">
+      <c r="A39" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="21.6" customHeight="1">
+      <c r="A40" s="14"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="24"/>
+    </row>
+    <row r="41" spans="1:7" ht="21.6">
+      <c r="A41" s="14"/>
+      <c r="B41" s="20">
+        <f>B37+1</f>
+        <v>28</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="20">
+        <f>D37+1</f>
+        <v>15</v>
+      </c>
+      <c r="E41" s="20">
+        <v>9</v>
+      </c>
+      <c r="F41" s="21"/>
+      <c r="G41" s="20"/>
+    </row>
+    <row r="42" spans="1:7" ht="21.6">
+      <c r="A42" s="14"/>
+      <c r="B42" s="20">
+        <f>B41+1</f>
+        <v>29</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="20">
+        <f>D41+1</f>
+        <v>16</v>
+      </c>
+      <c r="E42" s="20">
+        <v>9</v>
+      </c>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+    </row>
+    <row r="43" spans="1:7" ht="21.6">
+      <c r="A43" s="14"/>
+      <c r="B43" s="20">
+        <f t="shared" ref="B43:B47" si="7">B42+1</f>
+        <v>30</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="20">
+        <f t="shared" ref="D43:D47" si="8">D42+1</f>
+        <v>17</v>
+      </c>
+      <c r="E43" s="20">
+        <v>9</v>
+      </c>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+    </row>
+    <row r="44" spans="1:7" ht="21.6">
+      <c r="A44" s="14"/>
+      <c r="B44" s="20">
+        <f t="shared" si="7"/>
+        <v>31</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="20">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="E44" s="20">
+        <v>9</v>
+      </c>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+    </row>
+    <row r="45" spans="1:7" ht="21.6">
+      <c r="A45" s="14"/>
+      <c r="B45" s="20">
+        <f t="shared" si="7"/>
+        <v>32</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="20">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="E45" s="20">
+        <v>9</v>
+      </c>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+    </row>
+    <row r="46" spans="1:7" ht="21.6">
+      <c r="A46" s="14"/>
+      <c r="B46" s="20">
+        <f t="shared" si="7"/>
+        <v>33</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="20">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="E46" s="20">
+        <v>9</v>
+      </c>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+    </row>
+    <row r="47" spans="1:7" ht="21.6">
+      <c r="A47" s="14"/>
+      <c r="B47" s="20">
+        <f t="shared" si="7"/>
+        <v>34</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="20">
+        <f t="shared" si="8"/>
+        <v>21</v>
+      </c>
+      <c r="E47" s="20">
+        <v>9</v>
+      </c>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+    </row>
+    <row r="48" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A48" s="14"/>
+      <c r="B48" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="1">
+        <f>SUM(F41:F47)</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" ht="21.6">
+      <c r="A49" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="21.6" customHeight="1">
+      <c r="A50" s="14"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="24"/>
+    </row>
+    <row r="51" spans="1:7" ht="21.6">
+      <c r="A51" s="14"/>
+      <c r="B51" s="20">
+        <f>B47+1</f>
+        <v>35</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" s="20">
+        <f>D47+1</f>
+        <v>22</v>
+      </c>
+      <c r="E51" s="20">
+        <v>9</v>
+      </c>
+      <c r="F51" s="21"/>
+      <c r="G51" s="20"/>
+    </row>
+    <row r="52" spans="1:7" ht="21.6">
+      <c r="A52" s="14"/>
+      <c r="B52" s="20">
+        <f>B51+1</f>
+        <v>36</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="20">
+        <f>D51+1</f>
+        <v>23</v>
+      </c>
+      <c r="E52" s="20">
+        <v>9</v>
+      </c>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+    </row>
+    <row r="53" spans="1:7" ht="21.6">
+      <c r="A53" s="14"/>
+      <c r="B53" s="20">
+        <f t="shared" ref="B53:B57" si="9">B52+1</f>
+        <v>37</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="20">
+        <f t="shared" ref="D53:D57" si="10">D52+1</f>
+        <v>24</v>
+      </c>
+      <c r="E53" s="20">
+        <v>9</v>
+      </c>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+    </row>
+    <row r="54" spans="1:7" ht="21.6">
+      <c r="A54" s="14"/>
+      <c r="B54" s="20">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="20">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="E54" s="20">
+        <v>9</v>
+      </c>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+    </row>
+    <row r="55" spans="1:7" ht="21.6">
+      <c r="A55" s="14"/>
+      <c r="B55" s="20">
+        <f t="shared" si="9"/>
+        <v>39</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="20">
+        <f t="shared" si="10"/>
+        <v>26</v>
+      </c>
+      <c r="E55" s="20">
+        <v>9</v>
+      </c>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+    </row>
+    <row r="56" spans="1:7" ht="21.6">
+      <c r="A56" s="14"/>
+      <c r="B56" s="20">
+        <f t="shared" si="9"/>
+        <v>40</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="20">
+        <f t="shared" si="10"/>
+        <v>27</v>
+      </c>
+      <c r="E56" s="20">
+        <v>9</v>
+      </c>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+    </row>
+    <row r="57" spans="1:7" ht="21.6">
+      <c r="A57" s="14"/>
+      <c r="B57" s="20">
+        <f t="shared" si="9"/>
+        <v>41</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="20">
+        <f t="shared" si="10"/>
+        <v>28</v>
+      </c>
+      <c r="E57" s="20">
+        <v>9</v>
+      </c>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+    </row>
+    <row r="58" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A58" s="14"/>
+      <c r="B58" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="1">
+        <f>SUM(F51:F57)</f>
+        <v>0</v>
+      </c>
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="1:7" ht="21.6">
+      <c r="A59" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="21.6" customHeight="1">
+      <c r="A60" s="14"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="24"/>
+    </row>
+    <row r="61" spans="1:7" ht="21.6">
+      <c r="A61" s="14"/>
+      <c r="B61" s="20">
+        <f>B57+1</f>
+        <v>42</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61" s="20">
+        <f>D57+1</f>
+        <v>29</v>
+      </c>
+      <c r="E61" s="20">
+        <v>9</v>
+      </c>
+      <c r="F61" s="21"/>
+      <c r="G61" s="20"/>
+    </row>
+    <row r="62" spans="1:7" ht="21.6">
+      <c r="A62" s="14"/>
+      <c r="B62" s="20">
+        <f>B61+1</f>
+        <v>43</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="20">
+        <f>D61+1</f>
+        <v>30</v>
+      </c>
+      <c r="E62" s="20">
+        <v>9</v>
+      </c>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
+    </row>
+    <row r="63" spans="1:7" ht="21.6">
+      <c r="A63" s="14"/>
+      <c r="B63" s="20">
+        <f t="shared" ref="B63:B67" si="11">B62+1</f>
+        <v>44</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" s="20">
+        <v>1</v>
+      </c>
+      <c r="E63" s="20">
+        <v>10</v>
+      </c>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+    </row>
+    <row r="64" spans="1:7" ht="21.6">
+      <c r="A64" s="14"/>
+      <c r="B64" s="20">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="20">
+        <f t="shared" ref="D63:D67" si="12">D63+1</f>
+        <v>2</v>
+      </c>
+      <c r="E64" s="20">
+        <v>10</v>
+      </c>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
+    </row>
+    <row r="65" spans="1:7" ht="21.6">
+      <c r="A65" s="14"/>
+      <c r="B65" s="20">
+        <f t="shared" si="11"/>
+        <v>46</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="20">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="E65" s="20">
+        <v>10</v>
+      </c>
+      <c r="F65" s="22"/>
+      <c r="G65" s="22"/>
+    </row>
+    <row r="66" spans="1:7" ht="21.6">
+      <c r="A66" s="14"/>
+      <c r="B66" s="20">
+        <f t="shared" si="11"/>
+        <v>47</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="20">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="E66" s="20">
+        <v>10</v>
+      </c>
+      <c r="F66" s="22"/>
+      <c r="G66" s="22"/>
+    </row>
+    <row r="67" spans="1:7" ht="21.6">
+      <c r="A67" s="14"/>
+      <c r="B67" s="20">
+        <f t="shared" si="11"/>
+        <v>48</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="20">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="E67" s="20">
+        <v>10</v>
+      </c>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+    </row>
+    <row r="68" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A68" s="14"/>
+      <c r="B68" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="27"/>
+      <c r="F68" s="1">
+        <f>SUM(F61:F67)</f>
+        <v>0</v>
+      </c>
+      <c r="G68" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="20">
+    <mergeCell ref="A59:A68"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="A1:A9"/>
+    <mergeCell ref="A10:A19"/>
+    <mergeCell ref="A39:A48"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="A49:A58"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="A29:A38"/>
+    <mergeCell ref="A20:A28"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A11:A19"/>
     <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
week 5 report: update weekly_report.xlsx
</commit_message>
<xml_diff>
--- a/reports/weekly_report.xlsx
+++ b/reports/weekly_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
   <si>
     <t>ردیف</t>
   </si>
@@ -151,6 +151,29 @@
   <si>
     <t>باسمه تعالی
 با سلام احترام، تمام ۱۷۰ ویدیو تک قسمتی سایت مونگارد مشاهده و نکته برداری  و تمرین شد.</t>
+  </si>
+  <si>
+    <t>search about testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python testing </t>
+  </si>
+  <si>
+    <t>sart numpy toturial in w3school.com</t>
+  </si>
+  <si>
+    <t>contineu numpy and summerize</t>
+  </si>
+  <si>
+    <t>countineu on w3school.com self study</t>
+  </si>
+  <si>
+    <t>self study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">باسمه تعالی.
+سلام علیکم. با احترام، این هفته به دوره های تست نویسی و numpy سایت مونگارد تخصیص یافت. همچنین به صورت خودآموز از سایت w3school در حال کار با کتابخانه numpy هستم.  همچنین کدها در ریپازیتوری مرتب و آپدیت شدند. 
+ساعت های درج شده در جدول زیر بر اساس time tracker بوده ولی متاسفانه به دلیل مشکل داشتن سایت امکان گزارش گیری وجود ندارد. </t>
   </si>
 </sst>
 </file>
@@ -384,38 +407,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -431,10 +446,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -449,6 +464,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -458,7 +482,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -770,7 +793,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21.6">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="26" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -793,7 +816,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A2" s="19"/>
+      <c r="A2" s="27"/>
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -814,7 +837,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="21.6">
-      <c r="A3" s="19"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="3">
         <f>B2+1</f>
         <v>2</v>
@@ -837,7 +860,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="21.6">
-      <c r="A4" s="19"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B18" si="0">B3+1</f>
         <v>3</v>
@@ -860,7 +883,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="21.6">
-      <c r="A5" s="19"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -883,7 +906,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="129.6">
-      <c r="A6" s="19"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -906,7 +929,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="21.6">
-      <c r="A7" s="19"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -927,7 +950,7 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="108">
-      <c r="A8" s="19"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -950,13 +973,13 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="21.6">
-      <c r="A9" s="30"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="34"/>
       <c r="F9" s="5">
         <f>SUM(F2:F8)</f>
         <v>22</v>
@@ -964,7 +987,7 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="21.6">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -987,18 +1010,18 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="121.8" customHeight="1">
-      <c r="A11" s="14"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A12" s="14"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="1">
         <f>B8+1</f>
         <v>8</v>
@@ -1022,7 +1045,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="14"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1046,7 +1069,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="14"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1070,7 +1093,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="14"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1094,7 +1117,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="14"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1118,7 +1141,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="14"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1140,7 +1163,7 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="14"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1163,13 +1186,13 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="21.6">
-      <c r="A19" s="29"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34"/>
       <c r="F19" s="5">
         <f>SUM(F12:F18)</f>
         <v>15.5</v>
@@ -1177,7 +1200,7 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="21.6">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="15" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1200,18 +1223,18 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="152.4" customHeight="1">
-      <c r="A21" s="14"/>
-      <c r="B21" s="12" t="s">
+      <c r="A21" s="16"/>
+      <c r="B21" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A22" s="14"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="1">
         <f>B18+1</f>
         <v>15</v>
@@ -1235,7 +1258,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A23" s="14"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="1">
         <f>B22+1</f>
         <v>16</v>
@@ -1258,7 +1281,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A24" s="14"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="1">
         <f t="shared" ref="B24:B27" si="4">B23+1</f>
         <v>17</v>
@@ -1281,7 +1304,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A25" s="14"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="1">
         <f t="shared" si="4"/>
         <v>18</v>
@@ -1304,7 +1327,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A26" s="14"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="1">
         <f t="shared" si="4"/>
         <v>19</v>
@@ -1327,7 +1350,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A27" s="14"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="1">
         <f t="shared" si="4"/>
         <v>20</v>
@@ -1350,13 +1373,13 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="29"/>
-      <c r="B28" s="11" t="s">
+      <c r="A28" s="17"/>
+      <c r="B28" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
       <c r="F28" s="10">
         <f>SUM(F22:F27)</f>
         <v>26.15</v>
@@ -1364,7 +1387,7 @@
       <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:7" ht="21.6">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1387,191 +1410,191 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="40.200000000000003" customHeight="1">
-      <c r="A30" s="14"/>
-      <c r="B30" s="31" t="s">
+      <c r="A30" s="16"/>
+      <c r="B30" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="33"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="31"/>
     </row>
     <row r="31" spans="1:7" ht="21.6">
-      <c r="A31" s="14"/>
-      <c r="B31" s="20">
+      <c r="A31" s="16"/>
+      <c r="B31" s="11">
         <f>B27+1</f>
         <v>21</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="20">
+      <c r="D31" s="11">
         <f>D27+1</f>
         <v>8</v>
       </c>
-      <c r="E31" s="20">
-        <v>9</v>
-      </c>
-      <c r="F31" s="21">
+      <c r="E31" s="11">
+        <v>9</v>
+      </c>
+      <c r="F31" s="12">
         <v>2.25</v>
       </c>
-      <c r="G31" s="20" t="s">
+      <c r="G31" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="21.6">
-      <c r="A32" s="14"/>
-      <c r="B32" s="20">
+      <c r="A32" s="16"/>
+      <c r="B32" s="11">
         <f>B31+1</f>
         <v>22</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="20">
+      <c r="D32" s="11">
         <f>D31+1</f>
         <v>9</v>
       </c>
-      <c r="E32" s="20">
-        <v>9</v>
-      </c>
-      <c r="F32" s="22">
+      <c r="E32" s="11">
+        <v>9</v>
+      </c>
+      <c r="F32" s="13">
         <v>3.3</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G32" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="21.6">
-      <c r="A33" s="14"/>
-      <c r="B33" s="20">
+      <c r="A33" s="16"/>
+      <c r="B33" s="11">
         <f t="shared" ref="B33:B37" si="5">B32+1</f>
         <v>23</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="20">
+      <c r="D33" s="11">
         <f t="shared" ref="D33:D37" si="6">D32+1</f>
         <v>10</v>
       </c>
-      <c r="E33" s="20">
-        <v>9</v>
-      </c>
-      <c r="F33" s="22">
+      <c r="E33" s="11">
+        <v>9</v>
+      </c>
+      <c r="F33" s="13">
         <v>2.85</v>
       </c>
-      <c r="G33" s="22" t="s">
+      <c r="G33" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="21.6">
-      <c r="A34" s="14"/>
-      <c r="B34" s="20">
+      <c r="A34" s="16"/>
+      <c r="B34" s="11">
         <f t="shared" si="5"/>
         <v>24</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="20">
+      <c r="D34" s="11">
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
-      <c r="E34" s="20">
-        <v>9</v>
-      </c>
-      <c r="F34" s="22">
+      <c r="E34" s="11">
+        <v>9</v>
+      </c>
+      <c r="F34" s="13">
         <v>2.9</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="G34" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="21.6">
-      <c r="A35" s="14"/>
-      <c r="B35" s="20">
+      <c r="A35" s="16"/>
+      <c r="B35" s="11">
         <f t="shared" si="5"/>
         <v>25</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="20">
+      <c r="D35" s="11">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="E35" s="20">
-        <v>9</v>
-      </c>
-      <c r="F35" s="22">
+      <c r="E35" s="11">
+        <v>9</v>
+      </c>
+      <c r="F35" s="13">
         <v>0</v>
       </c>
-      <c r="G35" s="22"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:7" ht="21.6">
-      <c r="A36" s="14"/>
-      <c r="B36" s="20">
+      <c r="A36" s="16"/>
+      <c r="B36" s="11">
         <f t="shared" si="5"/>
         <v>26</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="20">
+      <c r="D36" s="11">
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="E36" s="20">
-        <v>9</v>
-      </c>
-      <c r="F36" s="22">
+      <c r="E36" s="11">
+        <v>9</v>
+      </c>
+      <c r="F36" s="13">
         <v>6.6</v>
       </c>
-      <c r="G36" s="22" t="s">
+      <c r="G36" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="21.6">
-      <c r="A37" s="14"/>
-      <c r="B37" s="20">
+      <c r="A37" s="16"/>
+      <c r="B37" s="11">
         <f t="shared" si="5"/>
         <v>27</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="20">
+      <c r="D37" s="11">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="E37" s="20">
-        <v>9</v>
-      </c>
-      <c r="F37" s="22">
+      <c r="E37" s="11">
+        <v>9</v>
+      </c>
+      <c r="F37" s="13">
         <v>1.9</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="G37" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A38" s="14"/>
-      <c r="B38" s="34" t="s">
+      <c r="A38" s="16"/>
+      <c r="B38" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="37">
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="14">
         <f>SUM(F31:F37)</f>
         <v>19.799999999999997</v>
       </c>
-      <c r="G38" s="37"/>
+      <c r="G38" s="14"/>
     </row>
     <row r="39" spans="1:7" ht="21.6">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="15" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -1593,164 +1616,194 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A40" s="14"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="24"/>
+    <row r="40" spans="1:7" ht="99.6" customHeight="1">
+      <c r="A40" s="16"/>
+      <c r="B40" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="31"/>
     </row>
     <row r="41" spans="1:7" ht="21.6">
-      <c r="A41" s="14"/>
-      <c r="B41" s="20">
+      <c r="A41" s="16"/>
+      <c r="B41" s="11">
         <f>B37+1</f>
         <v>28</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D41" s="20">
+      <c r="D41" s="11">
         <f>D37+1</f>
         <v>15</v>
       </c>
-      <c r="E41" s="20">
-        <v>9</v>
-      </c>
-      <c r="F41" s="21"/>
-      <c r="G41" s="20"/>
+      <c r="E41" s="11">
+        <v>9</v>
+      </c>
+      <c r="F41" s="12">
+        <v>5</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="21.6">
-      <c r="A42" s="14"/>
-      <c r="B42" s="20">
+      <c r="A42" s="16"/>
+      <c r="B42" s="11">
         <f>B41+1</f>
         <v>29</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="20">
+      <c r="D42" s="11">
         <f>D41+1</f>
         <v>16</v>
       </c>
-      <c r="E42" s="20">
-        <v>9</v>
-      </c>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
+      <c r="E42" s="11">
+        <v>9</v>
+      </c>
+      <c r="F42" s="13">
+        <v>1.9</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="21.6">
-      <c r="A43" s="14"/>
-      <c r="B43" s="20">
+      <c r="A43" s="16"/>
+      <c r="B43" s="11">
         <f t="shared" ref="B43:B47" si="7">B42+1</f>
         <v>30</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="20">
+      <c r="D43" s="11">
         <f t="shared" ref="D43:D47" si="8">D42+1</f>
         <v>17</v>
       </c>
-      <c r="E43" s="20">
-        <v>9</v>
-      </c>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
+      <c r="E43" s="11">
+        <v>9</v>
+      </c>
+      <c r="F43" s="13">
+        <v>1.8</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="21.6">
-      <c r="A44" s="14"/>
-      <c r="B44" s="20">
+      <c r="A44" s="16"/>
+      <c r="B44" s="11">
         <f t="shared" si="7"/>
         <v>31</v>
       </c>
-      <c r="C44" s="20" t="s">
+      <c r="C44" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="20">
+      <c r="D44" s="11">
         <f t="shared" si="8"/>
         <v>18</v>
       </c>
-      <c r="E44" s="20">
-        <v>9</v>
-      </c>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
+      <c r="E44" s="11">
+        <v>9</v>
+      </c>
+      <c r="F44" s="13">
+        <v>4.75</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="21.6">
-      <c r="A45" s="14"/>
-      <c r="B45" s="20">
+      <c r="A45" s="16"/>
+      <c r="B45" s="11">
         <f t="shared" si="7"/>
         <v>32</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C45" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="20">
+      <c r="D45" s="11">
         <f t="shared" si="8"/>
         <v>19</v>
       </c>
-      <c r="E45" s="20">
-        <v>9</v>
-      </c>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
+      <c r="E45" s="11">
+        <v>9</v>
+      </c>
+      <c r="F45" s="13">
+        <v>8</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="21.6">
-      <c r="A46" s="14"/>
-      <c r="B46" s="20">
+      <c r="A46" s="16"/>
+      <c r="B46" s="11">
         <f t="shared" si="7"/>
         <v>33</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="20">
+      <c r="D46" s="11">
         <f t="shared" si="8"/>
         <v>20</v>
       </c>
-      <c r="E46" s="20">
-        <v>9</v>
-      </c>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
+      <c r="E46" s="11">
+        <v>9</v>
+      </c>
+      <c r="F46" s="13">
+        <v>8</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="21.6">
-      <c r="A47" s="14"/>
-      <c r="B47" s="20">
+      <c r="A47" s="16"/>
+      <c r="B47" s="11">
         <f t="shared" si="7"/>
         <v>34</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="20">
+      <c r="D47" s="11">
         <f t="shared" si="8"/>
         <v>21</v>
       </c>
-      <c r="E47" s="20">
-        <v>9</v>
-      </c>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
+      <c r="E47" s="11">
+        <v>9</v>
+      </c>
+      <c r="F47" s="13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A48" s="14"/>
-      <c r="B48" s="25" t="s">
+      <c r="A48" s="16"/>
+      <c r="B48" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="25"/>
       <c r="F48" s="1">
         <f>SUM(F41:F47)</f>
-        <v>0</v>
+        <v>31.650000000000002</v>
       </c>
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" ht="21.6">
-      <c r="A49" s="28" t="s">
+      <c r="A49" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B49" s="7" t="s">
@@ -1773,155 +1826,155 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A50" s="14"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="24"/>
+      <c r="A50" s="16"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="22"/>
     </row>
     <row r="51" spans="1:7" ht="21.6">
-      <c r="A51" s="14"/>
-      <c r="B51" s="20">
+      <c r="A51" s="16"/>
+      <c r="B51" s="11">
         <f>B47+1</f>
         <v>35</v>
       </c>
-      <c r="C51" s="20" t="s">
+      <c r="C51" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="20">
+      <c r="D51" s="11">
         <f>D47+1</f>
         <v>22</v>
       </c>
-      <c r="E51" s="20">
-        <v>9</v>
-      </c>
-      <c r="F51" s="21"/>
-      <c r="G51" s="20"/>
+      <c r="E51" s="11">
+        <v>9</v>
+      </c>
+      <c r="F51" s="12"/>
+      <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" ht="21.6">
-      <c r="A52" s="14"/>
-      <c r="B52" s="20">
+      <c r="A52" s="16"/>
+      <c r="B52" s="11">
         <f>B51+1</f>
         <v>36</v>
       </c>
-      <c r="C52" s="20" t="s">
+      <c r="C52" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D52" s="20">
+      <c r="D52" s="11">
         <f>D51+1</f>
         <v>23</v>
       </c>
-      <c r="E52" s="20">
-        <v>9</v>
-      </c>
-      <c r="F52" s="22"/>
-      <c r="G52" s="22"/>
+      <c r="E52" s="11">
+        <v>9</v>
+      </c>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
     </row>
     <row r="53" spans="1:7" ht="21.6">
-      <c r="A53" s="14"/>
-      <c r="B53" s="20">
+      <c r="A53" s="16"/>
+      <c r="B53" s="11">
         <f t="shared" ref="B53:B57" si="9">B52+1</f>
         <v>37</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="20">
+      <c r="D53" s="11">
         <f t="shared" ref="D53:D57" si="10">D52+1</f>
         <v>24</v>
       </c>
-      <c r="E53" s="20">
-        <v>9</v>
-      </c>
-      <c r="F53" s="22"/>
-      <c r="G53" s="22"/>
+      <c r="E53" s="11">
+        <v>9</v>
+      </c>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
     </row>
     <row r="54" spans="1:7" ht="21.6">
-      <c r="A54" s="14"/>
-      <c r="B54" s="20">
+      <c r="A54" s="16"/>
+      <c r="B54" s="11">
         <f t="shared" si="9"/>
         <v>38</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="20">
+      <c r="D54" s="11">
         <f t="shared" si="10"/>
         <v>25</v>
       </c>
-      <c r="E54" s="20">
-        <v>9</v>
-      </c>
-      <c r="F54" s="22"/>
-      <c r="G54" s="22"/>
+      <c r="E54" s="11">
+        <v>9</v>
+      </c>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
     </row>
     <row r="55" spans="1:7" ht="21.6">
-      <c r="A55" s="14"/>
-      <c r="B55" s="20">
+      <c r="A55" s="16"/>
+      <c r="B55" s="11">
         <f t="shared" si="9"/>
         <v>39</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D55" s="20">
+      <c r="D55" s="11">
         <f t="shared" si="10"/>
         <v>26</v>
       </c>
-      <c r="E55" s="20">
-        <v>9</v>
-      </c>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
+      <c r="E55" s="11">
+        <v>9</v>
+      </c>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:7" ht="21.6">
-      <c r="A56" s="14"/>
-      <c r="B56" s="20">
+      <c r="A56" s="16"/>
+      <c r="B56" s="11">
         <f t="shared" si="9"/>
         <v>40</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="C56" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D56" s="20">
+      <c r="D56" s="11">
         <f t="shared" si="10"/>
         <v>27</v>
       </c>
-      <c r="E56" s="20">
-        <v>9</v>
-      </c>
-      <c r="F56" s="22"/>
-      <c r="G56" s="22"/>
+      <c r="E56" s="11">
+        <v>9</v>
+      </c>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:7" ht="21.6">
-      <c r="A57" s="14"/>
-      <c r="B57" s="20">
+      <c r="A57" s="16"/>
+      <c r="B57" s="11">
         <f t="shared" si="9"/>
         <v>41</v>
       </c>
-      <c r="C57" s="20" t="s">
+      <c r="C57" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="20">
+      <c r="D57" s="11">
         <f t="shared" si="10"/>
         <v>28</v>
       </c>
-      <c r="E57" s="20">
-        <v>9</v>
-      </c>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
+      <c r="E57" s="11">
+        <v>9</v>
+      </c>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A58" s="14"/>
-      <c r="B58" s="25" t="s">
+      <c r="A58" s="16"/>
+      <c r="B58" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="27"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="25"/>
       <c r="F58" s="1">
         <f>SUM(F51:F57)</f>
         <v>0</v>
@@ -1929,7 +1982,7 @@
       <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7" ht="21.6">
-      <c r="A59" s="28" t="s">
+      <c r="A59" s="15" t="s">
         <v>39</v>
       </c>
       <c r="B59" s="7" t="s">
@@ -1952,154 +2005,154 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A60" s="14"/>
-      <c r="B60" s="23"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="23"/>
-      <c r="E60" s="23"/>
-      <c r="F60" s="23"/>
-      <c r="G60" s="24"/>
+      <c r="A60" s="16"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="22"/>
     </row>
     <row r="61" spans="1:7" ht="21.6">
-      <c r="A61" s="14"/>
-      <c r="B61" s="20">
+      <c r="A61" s="16"/>
+      <c r="B61" s="11">
         <f>B57+1</f>
         <v>42</v>
       </c>
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D61" s="20">
+      <c r="D61" s="11">
         <f>D57+1</f>
         <v>29</v>
       </c>
-      <c r="E61" s="20">
-        <v>9</v>
-      </c>
-      <c r="F61" s="21"/>
-      <c r="G61" s="20"/>
+      <c r="E61" s="11">
+        <v>9</v>
+      </c>
+      <c r="F61" s="12"/>
+      <c r="G61" s="11"/>
     </row>
     <row r="62" spans="1:7" ht="21.6">
-      <c r="A62" s="14"/>
-      <c r="B62" s="20">
+      <c r="A62" s="16"/>
+      <c r="B62" s="11">
         <f>B61+1</f>
         <v>43</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="C62" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D62" s="20">
+      <c r="D62" s="11">
         <f>D61+1</f>
         <v>30</v>
       </c>
-      <c r="E62" s="20">
-        <v>9</v>
-      </c>
-      <c r="F62" s="22"/>
-      <c r="G62" s="22"/>
+      <c r="E62" s="11">
+        <v>9</v>
+      </c>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
     </row>
     <row r="63" spans="1:7" ht="21.6">
-      <c r="A63" s="14"/>
-      <c r="B63" s="20">
+      <c r="A63" s="16"/>
+      <c r="B63" s="11">
         <f t="shared" ref="B63:B67" si="11">B62+1</f>
         <v>44</v>
       </c>
-      <c r="C63" s="20" t="s">
+      <c r="C63" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D63" s="20">
+      <c r="D63" s="11">
         <v>1</v>
       </c>
-      <c r="E63" s="20">
+      <c r="E63" s="11">
         <v>10</v>
       </c>
-      <c r="F63" s="22"/>
-      <c r="G63" s="22"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
     </row>
     <row r="64" spans="1:7" ht="21.6">
-      <c r="A64" s="14"/>
-      <c r="B64" s="20">
+      <c r="A64" s="16"/>
+      <c r="B64" s="11">
         <f t="shared" si="11"/>
         <v>45</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D64" s="20">
-        <f t="shared" ref="D63:D67" si="12">D63+1</f>
+      <c r="D64" s="11">
+        <f t="shared" ref="D64:D67" si="12">D63+1</f>
         <v>2</v>
       </c>
-      <c r="E64" s="20">
+      <c r="E64" s="11">
         <v>10</v>
       </c>
-      <c r="F64" s="22"/>
-      <c r="G64" s="22"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
     </row>
     <row r="65" spans="1:7" ht="21.6">
-      <c r="A65" s="14"/>
-      <c r="B65" s="20">
+      <c r="A65" s="16"/>
+      <c r="B65" s="11">
         <f t="shared" si="11"/>
         <v>46</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D65" s="20">
+      <c r="D65" s="11">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="E65" s="20">
+      <c r="E65" s="11">
         <v>10</v>
       </c>
-      <c r="F65" s="22"/>
-      <c r="G65" s="22"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
     </row>
     <row r="66" spans="1:7" ht="21.6">
-      <c r="A66" s="14"/>
-      <c r="B66" s="20">
+      <c r="A66" s="16"/>
+      <c r="B66" s="11">
         <f t="shared" si="11"/>
         <v>47</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D66" s="20">
+      <c r="D66" s="11">
         <f t="shared" si="12"/>
         <v>4</v>
       </c>
-      <c r="E66" s="20">
+      <c r="E66" s="11">
         <v>10</v>
       </c>
-      <c r="F66" s="22"/>
-      <c r="G66" s="22"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
     </row>
     <row r="67" spans="1:7" ht="21.6">
-      <c r="A67" s="14"/>
-      <c r="B67" s="20">
+      <c r="A67" s="16"/>
+      <c r="B67" s="11">
         <f t="shared" si="11"/>
         <v>48</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D67" s="20">
+      <c r="D67" s="11">
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="E67" s="20">
+      <c r="E67" s="11">
         <v>10</v>
       </c>
-      <c r="F67" s="22"/>
-      <c r="G67" s="22"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
     </row>
     <row r="68" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A68" s="14"/>
-      <c r="B68" s="25" t="s">
+      <c r="A68" s="16"/>
+      <c r="B68" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C68" s="26"/>
-      <c r="D68" s="26"/>
-      <c r="E68" s="27"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="25"/>
       <c r="F68" s="1">
         <f>SUM(F61:F67)</f>
         <v>0</v>
@@ -2108,17 +2161,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A59:A68"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B68:E68"/>
     <mergeCell ref="A1:A9"/>
     <mergeCell ref="A10:A19"/>
     <mergeCell ref="A39:A48"/>
     <mergeCell ref="B40:G40"/>
     <mergeCell ref="B48:E48"/>
-    <mergeCell ref="A49:A58"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B58:E58"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B38:E38"/>
@@ -2128,6 +2175,12 @@
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A59:A68"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="A49:A58"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B58:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
week 6 report: update weekly_report.xlsx
</commit_message>
<xml_diff>
--- a/reports/weekly_report.xlsx
+++ b/reports/weekly_report.xlsx
@@ -1,20 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F1F290-8986-4F1B-8772-D3387750184C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="سید علی" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="58">
   <si>
     <t>ردیف</t>
   </si>
@@ -174,12 +189,36 @@
     <t xml:space="preserve">باسمه تعالی.
 سلام علیکم. با احترام، این هفته به دوره های تست نویسی و numpy سایت مونگارد تخصیص یافت. همچنین به صورت خودآموز از سایت w3school در حال کار با کتابخانه numpy هستم.  همچنین کدها در ریپازیتوری مرتب و آپدیت شدند. 
 ساعت های درج شده در جدول زیر بر اساس time tracker بوده ولی متاسفانه به دلیل مشکل داشتن سایت امکان گزارش گیری وجود ندارد. </t>
+  </si>
+  <si>
+    <t>study numpy</t>
+  </si>
+  <si>
+    <t>contineu on numpy</t>
+  </si>
+  <si>
+    <t>work with numpy</t>
+  </si>
+  <si>
+    <t>work with numpy AND start pandas</t>
+  </si>
+  <si>
+    <t>work with pandas</t>
+  </si>
+  <si>
+    <t>pandas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+با سمه نعالی 
+با سلام و احترام. این هفته صرف یادگیری، تمرین و کار با کتابخونه‌های numpy  و pandas شد.
+کد‌های پیاده سازی شده نیز در دایرکتوری \self_study قرار گرفت</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -413,6 +452,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -422,6 +470,42 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -435,51 +519,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -488,6 +527,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -534,7 +581,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -566,9 +613,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,6 +665,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -775,25 +858,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="67.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21.6">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:7" ht="34.799999999999997">
+      <c r="A1" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -816,7 +900,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A2" s="27"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -836,8 +920,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="21.6">
-      <c r="A3" s="27"/>
+    <row r="3" spans="1:7" ht="17.399999999999999">
+      <c r="A3" s="16"/>
       <c r="B3" s="3">
         <f>B2+1</f>
         <v>2</v>
@@ -859,8 +943,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="21.6">
-      <c r="A4" s="27"/>
+    <row r="4" spans="1:7" ht="17.399999999999999">
+      <c r="A4" s="16"/>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B18" si="0">B3+1</f>
         <v>3</v>
@@ -882,8 +966,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="21.6">
-      <c r="A5" s="27"/>
+    <row r="5" spans="1:7" ht="17.399999999999999">
+      <c r="A5" s="16"/>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -905,8 +989,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="129.6">
-      <c r="A6" s="27"/>
+    <row r="6" spans="1:7" ht="87">
+      <c r="A6" s="16"/>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -928,8 +1012,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="21.6">
-      <c r="A7" s="27"/>
+    <row r="7" spans="1:7" ht="17.399999999999999">
+      <c r="A7" s="16"/>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -949,8 +1033,8 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="108">
-      <c r="A8" s="27"/>
+    <row r="8" spans="1:7" ht="87">
+      <c r="A8" s="16"/>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -972,22 +1056,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="21.6">
-      <c r="A9" s="28"/>
-      <c r="B9" s="32" t="s">
+    <row r="9" spans="1:7" ht="17.399999999999999">
+      <c r="A9" s="17"/>
+      <c r="B9" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="34"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
       <c r="F9" s="5">
         <f>SUM(F2:F8)</f>
         <v>22</v>
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="21.6">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:7" ht="34.799999999999997">
+      <c r="A10" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1010,18 +1094,18 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="121.8" customHeight="1">
-      <c r="A11" s="16"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
     </row>
     <row r="12" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A12" s="16"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="1">
         <f>B8+1</f>
         <v>8</v>
@@ -1045,7 +1129,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="16"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1069,7 +1153,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="16"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1093,7 +1177,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="16"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1117,7 +1201,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="16"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1141,7 +1225,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="16"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1163,7 +1247,7 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="16"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1185,22 +1269,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="21.6">
-      <c r="A19" s="17"/>
-      <c r="B19" s="32" t="s">
+    <row r="19" spans="1:7" ht="17.399999999999999">
+      <c r="A19" s="20"/>
+      <c r="B19" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="34"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="5">
         <f>SUM(F12:F18)</f>
         <v>15.5</v>
       </c>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" ht="21.6">
-      <c r="A20" s="15" t="s">
+    <row r="20" spans="1:7" ht="34.799999999999997">
+      <c r="A20" s="18" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1223,18 +1307,18 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="152.4" customHeight="1">
-      <c r="A21" s="16"/>
-      <c r="B21" s="19" t="s">
+      <c r="A21" s="19"/>
+      <c r="B21" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
     </row>
     <row r="22" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A22" s="16"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="1">
         <f>B18+1</f>
         <v>15</v>
@@ -1258,7 +1342,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A23" s="16"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="1">
         <f>B22+1</f>
         <v>16</v>
@@ -1281,7 +1365,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A24" s="16"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="1">
         <f t="shared" ref="B24:B27" si="4">B23+1</f>
         <v>17</v>
@@ -1304,7 +1388,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A25" s="16"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="1">
         <f t="shared" si="4"/>
         <v>18</v>
@@ -1327,7 +1411,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A26" s="16"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="1">
         <f t="shared" si="4"/>
         <v>19</v>
@@ -1350,7 +1434,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A27" s="16"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="1">
         <f t="shared" si="4"/>
         <v>20</v>
@@ -1373,21 +1457,21 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="17"/>
-      <c r="B28" s="18" t="s">
+      <c r="A28" s="20"/>
+      <c r="B28" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
       <c r="F28" s="10">
         <f>SUM(F22:F27)</f>
         <v>26.15</v>
       </c>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7" ht="21.6">
-      <c r="A29" s="15" t="s">
+    <row r="29" spans="1:7" ht="34.799999999999997">
+      <c r="A29" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1409,19 +1493,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="40.200000000000003" customHeight="1">
-      <c r="A30" s="16"/>
-      <c r="B30" s="29" t="s">
+    <row r="30" spans="1:7" ht="46.8" customHeight="1">
+      <c r="A30" s="19"/>
+      <c r="B30" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="31"/>
-    </row>
-    <row r="31" spans="1:7" ht="21.6">
-      <c r="A31" s="16"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="23"/>
+    </row>
+    <row r="31" spans="1:7" ht="17.399999999999999">
+      <c r="A31" s="19"/>
       <c r="B31" s="11">
         <f>B27+1</f>
         <v>21</v>
@@ -1443,8 +1527,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="21.6">
-      <c r="A32" s="16"/>
+    <row r="32" spans="1:7" ht="17.399999999999999">
+      <c r="A32" s="19"/>
       <c r="B32" s="11">
         <f>B31+1</f>
         <v>22</v>
@@ -1466,8 +1550,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="21.6">
-      <c r="A33" s="16"/>
+    <row r="33" spans="1:7" ht="17.399999999999999">
+      <c r="A33" s="19"/>
       <c r="B33" s="11">
         <f t="shared" ref="B33:B37" si="5">B32+1</f>
         <v>23</v>
@@ -1489,8 +1573,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="21.6">
-      <c r="A34" s="16"/>
+    <row r="34" spans="1:7" ht="17.399999999999999">
+      <c r="A34" s="19"/>
       <c r="B34" s="11">
         <f t="shared" si="5"/>
         <v>24</v>
@@ -1512,8 +1596,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="21.6">
-      <c r="A35" s="16"/>
+    <row r="35" spans="1:7" ht="17.399999999999999">
+      <c r="A35" s="19"/>
       <c r="B35" s="11">
         <f t="shared" si="5"/>
         <v>25</v>
@@ -1533,8 +1617,8 @@
       </c>
       <c r="G35" s="13"/>
     </row>
-    <row r="36" spans="1:7" ht="21.6">
-      <c r="A36" s="16"/>
+    <row r="36" spans="1:7" ht="17.399999999999999">
+      <c r="A36" s="19"/>
       <c r="B36" s="11">
         <f t="shared" si="5"/>
         <v>26</v>
@@ -1556,8 +1640,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="21.6">
-      <c r="A37" s="16"/>
+    <row r="37" spans="1:7" ht="17.399999999999999">
+      <c r="A37" s="19"/>
       <c r="B37" s="11">
         <f t="shared" si="5"/>
         <v>27</v>
@@ -1580,21 +1664,21 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A38" s="16"/>
-      <c r="B38" s="35" t="s">
+      <c r="A38" s="19"/>
+      <c r="B38" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="37"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="32"/>
       <c r="F38" s="14">
         <f>SUM(F31:F37)</f>
         <v>19.799999999999997</v>
       </c>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="1:7" ht="21.6">
-      <c r="A39" s="15" t="s">
+    <row r="39" spans="1:7" ht="34.799999999999997">
+      <c r="A39" s="18" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -1617,18 +1701,18 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="99.6" customHeight="1">
-      <c r="A40" s="16"/>
-      <c r="B40" s="29" t="s">
+      <c r="A40" s="19"/>
+      <c r="B40" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="31"/>
-    </row>
-    <row r="41" spans="1:7" ht="21.6">
-      <c r="A41" s="16"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="23"/>
+    </row>
+    <row r="41" spans="1:7" ht="17.399999999999999">
+      <c r="A41" s="19"/>
       <c r="B41" s="11">
         <f>B37+1</f>
         <v>28</v>
@@ -1650,8 +1734,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="21.6">
-      <c r="A42" s="16"/>
+    <row r="42" spans="1:7" ht="17.399999999999999">
+      <c r="A42" s="19"/>
       <c r="B42" s="11">
         <f>B41+1</f>
         <v>29</v>
@@ -1673,8 +1757,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="21.6">
-      <c r="A43" s="16"/>
+    <row r="43" spans="1:7" ht="17.399999999999999">
+      <c r="A43" s="19"/>
       <c r="B43" s="11">
         <f t="shared" ref="B43:B47" si="7">B42+1</f>
         <v>30</v>
@@ -1696,8 +1780,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="21.6">
-      <c r="A44" s="16"/>
+    <row r="44" spans="1:7" ht="17.399999999999999">
+      <c r="A44" s="19"/>
       <c r="B44" s="11">
         <f t="shared" si="7"/>
         <v>31</v>
@@ -1719,8 +1803,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="21.6">
-      <c r="A45" s="16"/>
+    <row r="45" spans="1:7" ht="17.399999999999999">
+      <c r="A45" s="19"/>
       <c r="B45" s="11">
         <f t="shared" si="7"/>
         <v>32</v>
@@ -1742,8 +1826,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="21.6">
-      <c r="A46" s="16"/>
+    <row r="46" spans="1:7" ht="17.399999999999999">
+      <c r="A46" s="19"/>
       <c r="B46" s="11">
         <f t="shared" si="7"/>
         <v>33</v>
@@ -1765,8 +1849,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="21.6">
-      <c r="A47" s="16"/>
+    <row r="47" spans="1:7" ht="17.399999999999999">
+      <c r="A47" s="19"/>
       <c r="B47" s="11">
         <f t="shared" si="7"/>
         <v>34</v>
@@ -1789,21 +1873,21 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A48" s="16"/>
-      <c r="B48" s="23" t="s">
+      <c r="A48" s="19"/>
+      <c r="B48" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="26"/>
       <c r="F48" s="1">
         <f>SUM(F41:F47)</f>
         <v>31.650000000000002</v>
       </c>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" ht="21.6">
-      <c r="A49" s="15" t="s">
+    <row r="49" spans="1:7" ht="34.799999999999997">
+      <c r="A49" s="18" t="s">
         <v>38</v>
       </c>
       <c r="B49" s="7" t="s">
@@ -1821,21 +1905,23 @@
       <c r="F49" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G49" s="7" t="s">
+      <c r="G49" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A50" s="16"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="22"/>
-    </row>
-    <row r="51" spans="1:7" ht="21.6">
-      <c r="A51" s="16"/>
+    <row r="50" spans="1:7" ht="64.8" customHeight="1">
+      <c r="A50" s="19"/>
+      <c r="B50" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="23"/>
+    </row>
+    <row r="51" spans="1:7" ht="17.399999999999999">
+      <c r="A51" s="19"/>
       <c r="B51" s="11">
         <f>B47+1</f>
         <v>35</v>
@@ -1850,11 +1936,15 @@
       <c r="E51" s="11">
         <v>9</v>
       </c>
-      <c r="F51" s="12"/>
-      <c r="G51" s="11"/>
-    </row>
-    <row r="52" spans="1:7" ht="21.6">
-      <c r="A52" s="16"/>
+      <c r="F51" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="17.399999999999999">
+      <c r="A52" s="19"/>
       <c r="B52" s="11">
         <f>B51+1</f>
         <v>36</v>
@@ -1869,11 +1959,15 @@
       <c r="E52" s="11">
         <v>9</v>
       </c>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-    </row>
-    <row r="53" spans="1:7" ht="21.6">
-      <c r="A53" s="16"/>
+      <c r="F52" s="13">
+        <v>4.25</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="17.399999999999999">
+      <c r="A53" s="19"/>
       <c r="B53" s="11">
         <f t="shared" ref="B53:B57" si="9">B52+1</f>
         <v>37</v>
@@ -1888,11 +1982,15 @@
       <c r="E53" s="11">
         <v>9</v>
       </c>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-    </row>
-    <row r="54" spans="1:7" ht="21.6">
-      <c r="A54" s="16"/>
+      <c r="F53" s="13">
+        <v>4</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="17.399999999999999">
+      <c r="A54" s="19"/>
       <c r="B54" s="11">
         <f t="shared" si="9"/>
         <v>38</v>
@@ -1907,11 +2005,15 @@
       <c r="E54" s="11">
         <v>9</v>
       </c>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-    </row>
-    <row r="55" spans="1:7" ht="21.6">
-      <c r="A55" s="16"/>
+      <c r="F54" s="13">
+        <v>5.5</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="17.399999999999999">
+      <c r="A55" s="19"/>
       <c r="B55" s="11">
         <f t="shared" si="9"/>
         <v>39</v>
@@ -1926,11 +2028,15 @@
       <c r="E55" s="11">
         <v>9</v>
       </c>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-    </row>
-    <row r="56" spans="1:7" ht="21.6">
-      <c r="A56" s="16"/>
+      <c r="F55" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="17.399999999999999">
+      <c r="A56" s="19"/>
       <c r="B56" s="11">
         <f t="shared" si="9"/>
         <v>40</v>
@@ -1945,11 +2051,15 @@
       <c r="E56" s="11">
         <v>9</v>
       </c>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-    </row>
-    <row r="57" spans="1:7" ht="21.6">
-      <c r="A57" s="16"/>
+      <c r="F56" s="13">
+        <v>5.5</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="17.399999999999999">
+      <c r="A57" s="19"/>
       <c r="B57" s="11">
         <f t="shared" si="9"/>
         <v>41</v>
@@ -1964,25 +2074,29 @@
       <c r="E57" s="11">
         <v>9</v>
       </c>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
+      <c r="F57" s="13">
+        <v>3</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="58" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A58" s="16"/>
-      <c r="B58" s="23" t="s">
+      <c r="A58" s="19"/>
+      <c r="B58" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="25"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="26"/>
       <c r="F58" s="1">
         <f>SUM(F51:F57)</f>
-        <v>0</v>
+        <v>28.25</v>
       </c>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:7" ht="21.6">
-      <c r="A59" s="15" t="s">
+    <row r="59" spans="1:7" ht="34.799999999999997">
+      <c r="A59" s="18" t="s">
         <v>39</v>
       </c>
       <c r="B59" s="7" t="s">
@@ -2005,16 +2119,16 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A60" s="16"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
-      <c r="G60" s="22"/>
-    </row>
-    <row r="61" spans="1:7" ht="21.6">
-      <c r="A61" s="16"/>
+      <c r="A60" s="19"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="36"/>
+      <c r="G60" s="37"/>
+    </row>
+    <row r="61" spans="1:7" ht="17.399999999999999">
+      <c r="A61" s="19"/>
       <c r="B61" s="11">
         <f>B57+1</f>
         <v>42</v>
@@ -2032,8 +2146,8 @@
       <c r="F61" s="12"/>
       <c r="G61" s="11"/>
     </row>
-    <row r="62" spans="1:7" ht="21.6">
-      <c r="A62" s="16"/>
+    <row r="62" spans="1:7" ht="17.399999999999999">
+      <c r="A62" s="19"/>
       <c r="B62" s="11">
         <f>B61+1</f>
         <v>43</v>
@@ -2051,8 +2165,8 @@
       <c r="F62" s="13"/>
       <c r="G62" s="13"/>
     </row>
-    <row r="63" spans="1:7" ht="21.6">
-      <c r="A63" s="16"/>
+    <row r="63" spans="1:7" ht="17.399999999999999">
+      <c r="A63" s="19"/>
       <c r="B63" s="11">
         <f t="shared" ref="B63:B67" si="11">B62+1</f>
         <v>44</v>
@@ -2069,8 +2183,8 @@
       <c r="F63" s="13"/>
       <c r="G63" s="13"/>
     </row>
-    <row r="64" spans="1:7" ht="21.6">
-      <c r="A64" s="16"/>
+    <row r="64" spans="1:7" ht="17.399999999999999">
+      <c r="A64" s="19"/>
       <c r="B64" s="11">
         <f t="shared" si="11"/>
         <v>45</v>
@@ -2088,8 +2202,8 @@
       <c r="F64" s="13"/>
       <c r="G64" s="13"/>
     </row>
-    <row r="65" spans="1:7" ht="21.6">
-      <c r="A65" s="16"/>
+    <row r="65" spans="1:7" ht="17.399999999999999">
+      <c r="A65" s="19"/>
       <c r="B65" s="11">
         <f t="shared" si="11"/>
         <v>46</v>
@@ -2107,8 +2221,8 @@
       <c r="F65" s="13"/>
       <c r="G65" s="13"/>
     </row>
-    <row r="66" spans="1:7" ht="21.6">
-      <c r="A66" s="16"/>
+    <row r="66" spans="1:7" ht="17.399999999999999">
+      <c r="A66" s="19"/>
       <c r="B66" s="11">
         <f t="shared" si="11"/>
         <v>47</v>
@@ -2126,8 +2240,8 @@
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
     </row>
-    <row r="67" spans="1:7" ht="21.6">
-      <c r="A67" s="16"/>
+    <row r="67" spans="1:7" ht="17.399999999999999">
+      <c r="A67" s="19"/>
       <c r="B67" s="11">
         <f t="shared" si="11"/>
         <v>48</v>
@@ -2146,13 +2260,13 @@
       <c r="G67" s="13"/>
     </row>
     <row r="68" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A68" s="16"/>
-      <c r="B68" s="23" t="s">
+      <c r="A68" s="19"/>
+      <c r="B68" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="25"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="26"/>
       <c r="F68" s="1">
         <f>SUM(F61:F67)</f>
         <v>0</v>
@@ -2161,6 +2275,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A59:A68"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="A49:A58"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B58:E58"/>
     <mergeCell ref="A1:A9"/>
     <mergeCell ref="A10:A19"/>
     <mergeCell ref="A39:A48"/>
@@ -2175,12 +2295,6 @@
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A59:A68"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="A49:A58"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B58:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
week 7 report: update weekly_report.xlsx
</commit_message>
<xml_diff>
--- a/reports/weekly_report.xlsx
+++ b/reports/weekly_report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F1F290-8986-4F1B-8772-D3387750184C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3747C6F4-4A29-4540-9D20-5B7EEDD4D3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="62">
   <si>
     <t>ردیف</t>
   </si>
@@ -213,6 +213,19 @@
 با سمه نعالی 
 با سلام و احترام. این هفته صرف یادگیری، تمرین و کار با کتابخونه‌های numpy  و pandas شد.
 کد‌های پیاده سازی شده نیز در دایرکتوری \self_study قرار گرفت</t>
+  </si>
+  <si>
+    <t>some coding</t>
+  </si>
+  <si>
+    <t>anderstanding project</t>
+  </si>
+  <si>
+    <t>work on project</t>
+  </si>
+  <si>
+    <t>با سمه نعالی 
+با سلام و احترام. این هفته پروژه تا فاز 3.1 (پردازش chunk-based) پیش رفت.</t>
   </si>
 </sst>
 </file>
@@ -226,12 +239,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="B Nazanin"/>
-      <charset val="178"/>
     </font>
     <font>
       <sz val="14"/>
@@ -252,6 +259,12 @@
       <color theme="1"/>
       <name val="B Nazanin"/>
       <charset val="178"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="B Nazanin"/>
     </font>
   </fonts>
   <fills count="5">
@@ -432,94 +445,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -861,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -876,8 +889,8 @@
     <col min="7" max="7" width="67.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="34.799999999999997">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7" ht="17.399999999999999">
+      <c r="A1" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -900,7 +913,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A2" s="16"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -921,7 +934,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.399999999999999">
-      <c r="A3" s="16"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="3">
         <f>B2+1</f>
         <v>2</v>
@@ -944,7 +957,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.399999999999999">
-      <c r="A4" s="16"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B18" si="0">B3+1</f>
         <v>3</v>
@@ -967,7 +980,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.399999999999999">
-      <c r="A5" s="16"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -990,7 +1003,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="87">
-      <c r="A6" s="16"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1013,7 +1026,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="17.399999999999999">
-      <c r="A7" s="16"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1034,7 +1047,7 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="87">
-      <c r="A8" s="16"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1057,7 +1070,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.399999999999999">
-      <c r="A9" s="17"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="27" t="s">
         <v>18</v>
       </c>
@@ -1070,8 +1083,8 @@
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="34.799999999999997">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:7" ht="17.399999999999999">
+      <c r="A10" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1094,7 +1107,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="121.8" customHeight="1">
-      <c r="A11" s="19"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="34" t="s">
         <v>26</v>
       </c>
@@ -1105,7 +1118,7 @@
       <c r="G11" s="35"/>
     </row>
     <row r="12" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A12" s="19"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="1">
         <f>B8+1</f>
         <v>8</v>
@@ -1129,7 +1142,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="19"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1153,7 +1166,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="19"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1177,7 +1190,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="19"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1201,7 +1214,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="19"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1225,7 +1238,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="19"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1247,7 +1260,7 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="19"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1270,7 +1283,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="17.399999999999999">
-      <c r="A19" s="20"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="27" t="s">
         <v>18</v>
       </c>
@@ -1283,8 +1296,8 @@
       </c>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" ht="34.799999999999997">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:7" ht="17.399999999999999">
+      <c r="A20" s="15" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1307,7 +1320,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="152.4" customHeight="1">
-      <c r="A21" s="19"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="34" t="s">
         <v>33</v>
       </c>
@@ -1318,7 +1331,7 @@
       <c r="G21" s="35"/>
     </row>
     <row r="22" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A22" s="19"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="1">
         <f>B18+1</f>
         <v>15</v>
@@ -1342,7 +1355,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A23" s="19"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="1">
         <f>B22+1</f>
         <v>16</v>
@@ -1365,7 +1378,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A24" s="19"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="1">
         <f t="shared" ref="B24:B27" si="4">B23+1</f>
         <v>17</v>
@@ -1388,7 +1401,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A25" s="19"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="1">
         <f t="shared" si="4"/>
         <v>18</v>
@@ -1411,7 +1424,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A26" s="19"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="1">
         <f t="shared" si="4"/>
         <v>19</v>
@@ -1434,7 +1447,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A27" s="19"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="1">
         <f t="shared" si="4"/>
         <v>20</v>
@@ -1457,7 +1470,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="20"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="33" t="s">
         <v>18</v>
       </c>
@@ -1470,8 +1483,8 @@
       </c>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7" ht="34.799999999999997">
-      <c r="A29" s="18" t="s">
+    <row r="29" spans="1:7" ht="17.399999999999999">
+      <c r="A29" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1494,18 +1507,18 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="46.8" customHeight="1">
-      <c r="A30" s="19"/>
-      <c r="B30" s="21" t="s">
+      <c r="A30" s="16"/>
+      <c r="B30" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="23"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="22"/>
     </row>
     <row r="31" spans="1:7" ht="17.399999999999999">
-      <c r="A31" s="19"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="11">
         <f>B27+1</f>
         <v>21</v>
@@ -1528,7 +1541,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="17.399999999999999">
-      <c r="A32" s="19"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="11">
         <f>B31+1</f>
         <v>22</v>
@@ -1551,7 +1564,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="17.399999999999999">
-      <c r="A33" s="19"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="11">
         <f t="shared" ref="B33:B37" si="5">B32+1</f>
         <v>23</v>
@@ -1574,7 +1587,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="17.399999999999999">
-      <c r="A34" s="19"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="11">
         <f t="shared" si="5"/>
         <v>24</v>
@@ -1597,7 +1610,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="17.399999999999999">
-      <c r="A35" s="19"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="11">
         <f t="shared" si="5"/>
         <v>25</v>
@@ -1618,7 +1631,7 @@
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:7" ht="17.399999999999999">
-      <c r="A36" s="19"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="11">
         <f t="shared" si="5"/>
         <v>26</v>
@@ -1641,7 +1654,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="17.399999999999999">
-      <c r="A37" s="19"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="11">
         <f t="shared" si="5"/>
         <v>27</v>
@@ -1664,7 +1677,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A38" s="19"/>
+      <c r="A38" s="16"/>
       <c r="B38" s="30" t="s">
         <v>18</v>
       </c>
@@ -1677,8 +1690,8 @@
       </c>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="1:7" ht="34.799999999999997">
-      <c r="A39" s="18" t="s">
+    <row r="39" spans="1:7" ht="17.399999999999999">
+      <c r="A39" s="15" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -1701,18 +1714,18 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="99.6" customHeight="1">
-      <c r="A40" s="19"/>
-      <c r="B40" s="21" t="s">
+      <c r="A40" s="16"/>
+      <c r="B40" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="23"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="1:7" ht="17.399999999999999">
-      <c r="A41" s="19"/>
+      <c r="A41" s="16"/>
       <c r="B41" s="11">
         <f>B37+1</f>
         <v>28</v>
@@ -1735,7 +1748,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="17.399999999999999">
-      <c r="A42" s="19"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="11">
         <f>B41+1</f>
         <v>29</v>
@@ -1758,7 +1771,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="17.399999999999999">
-      <c r="A43" s="19"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="11">
         <f t="shared" ref="B43:B47" si="7">B42+1</f>
         <v>30</v>
@@ -1781,7 +1794,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="17.399999999999999">
-      <c r="A44" s="19"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="11">
         <f t="shared" si="7"/>
         <v>31</v>
@@ -1804,7 +1817,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="17.399999999999999">
-      <c r="A45" s="19"/>
+      <c r="A45" s="16"/>
       <c r="B45" s="11">
         <f t="shared" si="7"/>
         <v>32</v>
@@ -1827,7 +1840,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="17.399999999999999">
-      <c r="A46" s="19"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="11">
         <f t="shared" si="7"/>
         <v>33</v>
@@ -1850,7 +1863,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="17.399999999999999">
-      <c r="A47" s="19"/>
+      <c r="A47" s="16"/>
       <c r="B47" s="11">
         <f t="shared" si="7"/>
         <v>34</v>
@@ -1873,21 +1886,21 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A48" s="19"/>
-      <c r="B48" s="24" t="s">
+      <c r="A48" s="16"/>
+      <c r="B48" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="26"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="19"/>
       <c r="F48" s="1">
         <f>SUM(F41:F47)</f>
         <v>31.650000000000002</v>
       </c>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" ht="34.799999999999997">
-      <c r="A49" s="18" t="s">
+    <row r="49" spans="1:7" ht="17.399999999999999">
+      <c r="A49" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B49" s="7" t="s">
@@ -1910,18 +1923,18 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="64.8" customHeight="1">
-      <c r="A50" s="19"/>
-      <c r="B50" s="21" t="s">
+      <c r="A50" s="16"/>
+      <c r="B50" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="23"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="22"/>
     </row>
     <row r="51" spans="1:7" ht="17.399999999999999">
-      <c r="A51" s="19"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="11">
         <f>B47+1</f>
         <v>35</v>
@@ -1944,7 +1957,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="17.399999999999999">
-      <c r="A52" s="19"/>
+      <c r="A52" s="16"/>
       <c r="B52" s="11">
         <f>B51+1</f>
         <v>36</v>
@@ -1967,7 +1980,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" ht="17.399999999999999">
-      <c r="A53" s="19"/>
+      <c r="A53" s="16"/>
       <c r="B53" s="11">
         <f t="shared" ref="B53:B57" si="9">B52+1</f>
         <v>37</v>
@@ -1990,7 +2003,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="17.399999999999999">
-      <c r="A54" s="19"/>
+      <c r="A54" s="16"/>
       <c r="B54" s="11">
         <f t="shared" si="9"/>
         <v>38</v>
@@ -2013,7 +2026,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="17.399999999999999">
-      <c r="A55" s="19"/>
+      <c r="A55" s="16"/>
       <c r="B55" s="11">
         <f t="shared" si="9"/>
         <v>39</v>
@@ -2036,7 +2049,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="17.399999999999999">
-      <c r="A56" s="19"/>
+      <c r="A56" s="16"/>
       <c r="B56" s="11">
         <f t="shared" si="9"/>
         <v>40</v>
@@ -2059,7 +2072,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="17.399999999999999">
-      <c r="A57" s="19"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="11">
         <f t="shared" si="9"/>
         <v>41</v>
@@ -2082,21 +2095,21 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A58" s="19"/>
-      <c r="B58" s="24" t="s">
+      <c r="A58" s="16"/>
+      <c r="B58" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="26"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="19"/>
       <c r="F58" s="1">
         <f>SUM(F51:F57)</f>
         <v>28.25</v>
       </c>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:7" ht="34.799999999999997">
-      <c r="A59" s="18" t="s">
+    <row r="59" spans="1:7" ht="17.399999999999999">
+      <c r="A59" s="15" t="s">
         <v>39</v>
       </c>
       <c r="B59" s="7" t="s">
@@ -2119,16 +2132,18 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A60" s="19"/>
-      <c r="B60" s="36"/>
+      <c r="A60" s="16"/>
+      <c r="B60" s="36" t="s">
+        <v>61</v>
+      </c>
       <c r="C60" s="36"/>
       <c r="D60" s="36"/>
       <c r="E60" s="36"/>
       <c r="F60" s="36"/>
       <c r="G60" s="37"/>
     </row>
-    <row r="61" spans="1:7" ht="17.399999999999999">
-      <c r="A61" s="19"/>
+    <row r="61" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A61" s="16"/>
       <c r="B61" s="11">
         <f>B57+1</f>
         <v>42</v>
@@ -2143,11 +2158,15 @@
       <c r="E61" s="11">
         <v>9</v>
       </c>
-      <c r="F61" s="12"/>
-      <c r="G61" s="11"/>
-    </row>
-    <row r="62" spans="1:7" ht="17.399999999999999">
-      <c r="A62" s="19"/>
+      <c r="F61" s="12">
+        <v>2</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A62" s="16"/>
       <c r="B62" s="11">
         <f>B61+1</f>
         <v>43</v>
@@ -2162,11 +2181,15 @@
       <c r="E62" s="11">
         <v>9</v>
       </c>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-    </row>
-    <row r="63" spans="1:7" ht="17.399999999999999">
-      <c r="A63" s="19"/>
+      <c r="F62" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A63" s="16"/>
       <c r="B63" s="11">
         <f t="shared" ref="B63:B67" si="11">B62+1</f>
         <v>44</v>
@@ -2180,11 +2203,15 @@
       <c r="E63" s="11">
         <v>10</v>
       </c>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
+      <c r="F63" s="13">
+        <v>4</v>
+      </c>
+      <c r="G63" s="13" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="64" spans="1:7" ht="17.399999999999999">
-      <c r="A64" s="19"/>
+      <c r="A64" s="16"/>
       <c r="B64" s="11">
         <f t="shared" si="11"/>
         <v>45</v>
@@ -2199,11 +2226,15 @@
       <c r="E64" s="11">
         <v>10</v>
       </c>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
+      <c r="F64" s="13">
+        <v>5.5</v>
+      </c>
+      <c r="G64" s="13" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="65" spans="1:7" ht="17.399999999999999">
-      <c r="A65" s="19"/>
+      <c r="A65" s="16"/>
       <c r="B65" s="11">
         <f t="shared" si="11"/>
         <v>46</v>
@@ -2218,11 +2249,15 @@
       <c r="E65" s="11">
         <v>10</v>
       </c>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
+      <c r="F65" s="13">
+        <v>7.75</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="66" spans="1:7" ht="17.399999999999999">
-      <c r="A66" s="19"/>
+      <c r="A66" s="16"/>
       <c r="B66" s="11">
         <f t="shared" si="11"/>
         <v>47</v>
@@ -2237,11 +2272,13 @@
       <c r="E66" s="11">
         <v>10</v>
       </c>
-      <c r="F66" s="13"/>
+      <c r="F66" s="13">
+        <v>0</v>
+      </c>
       <c r="G66" s="13"/>
     </row>
     <row r="67" spans="1:7" ht="17.399999999999999">
-      <c r="A67" s="19"/>
+      <c r="A67" s="16"/>
       <c r="B67" s="11">
         <f t="shared" si="11"/>
         <v>48</v>
@@ -2256,31 +2293,29 @@
       <c r="E67" s="11">
         <v>10</v>
       </c>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
+      <c r="F67" s="13">
+        <v>7</v>
+      </c>
+      <c r="G67" s="13" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="68" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A68" s="19"/>
-      <c r="B68" s="24" t="s">
+      <c r="A68" s="16"/>
+      <c r="B68" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="26"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="19"/>
       <c r="F68" s="1">
         <f>SUM(F61:F67)</f>
-        <v>0</v>
+        <v>27.75</v>
       </c>
       <c r="G68" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A59:A68"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="A49:A58"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B58:E58"/>
     <mergeCell ref="A1:A9"/>
     <mergeCell ref="A10:A19"/>
     <mergeCell ref="A39:A48"/>
@@ -2295,6 +2330,12 @@
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A59:A68"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="A49:A58"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B58:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
week 8 report: update weekly_report.xlsx
</commit_message>
<xml_diff>
--- a/reports/weekly_report.xlsx
+++ b/reports/weekly_report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3747C6F4-4A29-4540-9D20-5B7EEDD4D3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804590C3-A426-4ADB-AE67-95C4A158D078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
   <si>
     <t>ردیف</t>
   </si>
@@ -224,7 +224,14 @@
     <t>work on project</t>
   </si>
   <si>
+    <t>هفته هشتم</t>
+  </si>
+  <si>
     <t>با سمه نعالی 
+با سلام و احترام. این هفته پروژه تا سر فاز 6 (rule Engine) یش رفت.</t>
+  </si>
+  <si>
+    <t>باسمه تعالی 
 با سلام و احترام. این هفته پروژه تا فاز 3.1 (پردازش chunk-based) پیش رفت.</t>
   </si>
 </sst>
@@ -465,12 +472,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -479,27 +507,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -872,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70:G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -890,7 +897,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17.399999999999999">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -913,7 +920,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A2" s="24"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -934,7 +941,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.399999999999999">
-      <c r="A3" s="24"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="3">
         <f>B2+1</f>
         <v>2</v>
@@ -957,7 +964,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.399999999999999">
-      <c r="A4" s="24"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B18" si="0">B3+1</f>
         <v>3</v>
@@ -980,7 +987,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.399999999999999">
-      <c r="A5" s="24"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1003,7 +1010,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="87">
-      <c r="A6" s="24"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1026,7 +1033,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="17.399999999999999">
-      <c r="A7" s="24"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1047,7 +1054,7 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="87">
-      <c r="A8" s="24"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1070,7 +1077,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.399999999999999">
-      <c r="A9" s="25"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="27" t="s">
         <v>18</v>
       </c>
@@ -1084,7 +1091,7 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="17.399999999999999">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1107,7 +1114,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="121.8" customHeight="1">
-      <c r="A11" s="16"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="34" t="s">
         <v>26</v>
       </c>
@@ -1118,7 +1125,7 @@
       <c r="G11" s="35"/>
     </row>
     <row r="12" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A12" s="16"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="1">
         <f>B8+1</f>
         <v>8</v>
@@ -1142,7 +1149,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="16"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1166,7 +1173,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="16"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1190,7 +1197,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="16"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1214,7 +1221,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="16"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1238,7 +1245,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="16"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1260,7 +1267,7 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="16"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1283,7 +1290,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="17.399999999999999">
-      <c r="A19" s="26"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="27" t="s">
         <v>18</v>
       </c>
@@ -1297,7 +1304,7 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="17.399999999999999">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="18" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1320,7 +1327,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="152.4" customHeight="1">
-      <c r="A21" s="16"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="34" t="s">
         <v>33</v>
       </c>
@@ -1331,7 +1338,7 @@
       <c r="G21" s="35"/>
     </row>
     <row r="22" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A22" s="16"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="1">
         <f>B18+1</f>
         <v>15</v>
@@ -1355,7 +1362,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A23" s="16"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="1">
         <f>B22+1</f>
         <v>16</v>
@@ -1378,7 +1385,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A24" s="16"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="1">
         <f t="shared" ref="B24:B27" si="4">B23+1</f>
         <v>17</v>
@@ -1401,7 +1408,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A25" s="16"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="1">
         <f t="shared" si="4"/>
         <v>18</v>
@@ -1424,7 +1431,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A26" s="16"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="1">
         <f t="shared" si="4"/>
         <v>19</v>
@@ -1447,7 +1454,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A27" s="16"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="1">
         <f t="shared" si="4"/>
         <v>20</v>
@@ -1470,7 +1477,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="26"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="33" t="s">
         <v>18</v>
       </c>
@@ -1484,7 +1491,7 @@
       <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:7" ht="17.399999999999999">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1507,18 +1514,18 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="46.8" customHeight="1">
-      <c r="A30" s="16"/>
-      <c r="B30" s="20" t="s">
+      <c r="A30" s="19"/>
+      <c r="B30" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="23"/>
     </row>
     <row r="31" spans="1:7" ht="17.399999999999999">
-      <c r="A31" s="16"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="11">
         <f>B27+1</f>
         <v>21</v>
@@ -1541,7 +1548,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="17.399999999999999">
-      <c r="A32" s="16"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="11">
         <f>B31+1</f>
         <v>22</v>
@@ -1564,7 +1571,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="17.399999999999999">
-      <c r="A33" s="16"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="11">
         <f t="shared" ref="B33:B37" si="5">B32+1</f>
         <v>23</v>
@@ -1587,7 +1594,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="17.399999999999999">
-      <c r="A34" s="16"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="11">
         <f t="shared" si="5"/>
         <v>24</v>
@@ -1610,7 +1617,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="17.399999999999999">
-      <c r="A35" s="16"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="11">
         <f t="shared" si="5"/>
         <v>25</v>
@@ -1631,7 +1638,7 @@
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:7" ht="17.399999999999999">
-      <c r="A36" s="16"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="11">
         <f t="shared" si="5"/>
         <v>26</v>
@@ -1654,7 +1661,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="17.399999999999999">
-      <c r="A37" s="16"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="11">
         <f t="shared" si="5"/>
         <v>27</v>
@@ -1677,7 +1684,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A38" s="16"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="30" t="s">
         <v>18</v>
       </c>
@@ -1691,7 +1698,7 @@
       <c r="G38" s="14"/>
     </row>
     <row r="39" spans="1:7" ht="17.399999999999999">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="18" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -1714,18 +1721,18 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="99.6" customHeight="1">
-      <c r="A40" s="16"/>
-      <c r="B40" s="20" t="s">
+      <c r="A40" s="19"/>
+      <c r="B40" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="23"/>
     </row>
     <row r="41" spans="1:7" ht="17.399999999999999">
-      <c r="A41" s="16"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="11">
         <f>B37+1</f>
         <v>28</v>
@@ -1748,7 +1755,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="17.399999999999999">
-      <c r="A42" s="16"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="11">
         <f>B41+1</f>
         <v>29</v>
@@ -1771,7 +1778,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="17.399999999999999">
-      <c r="A43" s="16"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="11">
         <f t="shared" ref="B43:B47" si="7">B42+1</f>
         <v>30</v>
@@ -1794,7 +1801,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="17.399999999999999">
-      <c r="A44" s="16"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="11">
         <f t="shared" si="7"/>
         <v>31</v>
@@ -1817,7 +1824,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="17.399999999999999">
-      <c r="A45" s="16"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="11">
         <f t="shared" si="7"/>
         <v>32</v>
@@ -1840,7 +1847,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="17.399999999999999">
-      <c r="A46" s="16"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="11">
         <f t="shared" si="7"/>
         <v>33</v>
@@ -1863,7 +1870,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="17.399999999999999">
-      <c r="A47" s="16"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="11">
         <f t="shared" si="7"/>
         <v>34</v>
@@ -1886,13 +1893,13 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A48" s="16"/>
-      <c r="B48" s="17" t="s">
+      <c r="A48" s="19"/>
+      <c r="B48" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="19"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="26"/>
       <c r="F48" s="1">
         <f>SUM(F41:F47)</f>
         <v>31.650000000000002</v>
@@ -1900,7 +1907,7 @@
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" ht="17.399999999999999">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="18" t="s">
         <v>38</v>
       </c>
       <c r="B49" s="7" t="s">
@@ -1923,18 +1930,18 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="64.8" customHeight="1">
-      <c r="A50" s="16"/>
-      <c r="B50" s="20" t="s">
+      <c r="A50" s="19"/>
+      <c r="B50" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="23"/>
     </row>
     <row r="51" spans="1:7" ht="17.399999999999999">
-      <c r="A51" s="16"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="11">
         <f>B47+1</f>
         <v>35</v>
@@ -1957,7 +1964,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="17.399999999999999">
-      <c r="A52" s="16"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="11">
         <f>B51+1</f>
         <v>36</v>
@@ -1980,7 +1987,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" ht="17.399999999999999">
-      <c r="A53" s="16"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="11">
         <f t="shared" ref="B53:B57" si="9">B52+1</f>
         <v>37</v>
@@ -2003,7 +2010,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="17.399999999999999">
-      <c r="A54" s="16"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="11">
         <f t="shared" si="9"/>
         <v>38</v>
@@ -2026,7 +2033,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="17.399999999999999">
-      <c r="A55" s="16"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="11">
         <f t="shared" si="9"/>
         <v>39</v>
@@ -2049,7 +2056,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="17.399999999999999">
-      <c r="A56" s="16"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="11">
         <f t="shared" si="9"/>
         <v>40</v>
@@ -2072,7 +2079,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="17.399999999999999">
-      <c r="A57" s="16"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="11">
         <f t="shared" si="9"/>
         <v>41</v>
@@ -2095,13 +2102,13 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A58" s="16"/>
-      <c r="B58" s="17" t="s">
+      <c r="A58" s="19"/>
+      <c r="B58" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="19"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="26"/>
       <c r="F58" s="1">
         <f>SUM(F51:F57)</f>
         <v>28.25</v>
@@ -2109,7 +2116,7 @@
       <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7" ht="17.399999999999999">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="18" t="s">
         <v>39</v>
       </c>
       <c r="B59" s="7" t="s">
@@ -2131,10 +2138,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A60" s="16"/>
+    <row r="60" spans="1:7" ht="42" customHeight="1">
+      <c r="A60" s="19"/>
       <c r="B60" s="36" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C60" s="36"/>
       <c r="D60" s="36"/>
@@ -2143,7 +2150,7 @@
       <c r="G60" s="37"/>
     </row>
     <row r="61" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A61" s="16"/>
+      <c r="A61" s="19"/>
       <c r="B61" s="11">
         <f>B57+1</f>
         <v>42</v>
@@ -2166,7 +2173,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A62" s="16"/>
+      <c r="A62" s="19"/>
       <c r="B62" s="11">
         <f>B61+1</f>
         <v>43</v>
@@ -2189,7 +2196,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A63" s="16"/>
+      <c r="A63" s="19"/>
       <c r="B63" s="11">
         <f t="shared" ref="B63:B67" si="11">B62+1</f>
         <v>44</v>
@@ -2211,7 +2218,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="17.399999999999999">
-      <c r="A64" s="16"/>
+      <c r="A64" s="19"/>
       <c r="B64" s="11">
         <f t="shared" si="11"/>
         <v>45</v>
@@ -2234,7 +2241,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="17.399999999999999">
-      <c r="A65" s="16"/>
+      <c r="A65" s="19"/>
       <c r="B65" s="11">
         <f t="shared" si="11"/>
         <v>46</v>
@@ -2257,7 +2264,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="17.399999999999999">
-      <c r="A66" s="16"/>
+      <c r="A66" s="19"/>
       <c r="B66" s="11">
         <f t="shared" si="11"/>
         <v>47</v>
@@ -2278,7 +2285,7 @@
       <c r="G66" s="13"/>
     </row>
     <row r="67" spans="1:7" ht="17.399999999999999">
-      <c r="A67" s="16"/>
+      <c r="A67" s="19"/>
       <c r="B67" s="11">
         <f t="shared" si="11"/>
         <v>48</v>
@@ -2301,21 +2308,235 @@
       </c>
     </row>
     <row r="68" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A68" s="16"/>
-      <c r="B68" s="17" t="s">
+      <c r="A68" s="19"/>
+      <c r="B68" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="19"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="26"/>
       <c r="F68" s="1">
         <f>SUM(F61:F67)</f>
         <v>27.75</v>
       </c>
       <c r="G68" s="1"/>
     </row>
+    <row r="69" spans="1:7" ht="17.399999999999999">
+      <c r="A69" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="40.200000000000003" customHeight="1">
+      <c r="A70" s="19"/>
+      <c r="B70" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C70" s="36"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="36"/>
+      <c r="F70" s="36"/>
+      <c r="G70" s="37"/>
+    </row>
+    <row r="71" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A71" s="19"/>
+      <c r="B71" s="11">
+        <f>B67+1</f>
+        <v>49</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D71" s="11">
+        <f>D67+1</f>
+        <v>6</v>
+      </c>
+      <c r="E71" s="11">
+        <v>10</v>
+      </c>
+      <c r="F71" s="12">
+        <v>4</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A72" s="19"/>
+      <c r="B72" s="11">
+        <f>B71+1</f>
+        <v>50</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="11">
+        <f>D71+1</f>
+        <v>7</v>
+      </c>
+      <c r="E72" s="11">
+        <v>10</v>
+      </c>
+      <c r="F72" s="13">
+        <v>5.25</v>
+      </c>
+      <c r="G72" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A73" s="19"/>
+      <c r="B73" s="11">
+        <f t="shared" ref="B73:B77" si="13">B72+1</f>
+        <v>51</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="11">
+        <f>D72+1</f>
+        <v>8</v>
+      </c>
+      <c r="E73" s="11">
+        <v>10</v>
+      </c>
+      <c r="F73" s="13">
+        <v>6.5</v>
+      </c>
+      <c r="G73" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="17.399999999999999">
+      <c r="A74" s="19"/>
+      <c r="B74" s="11">
+        <f t="shared" si="13"/>
+        <v>52</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" s="11">
+        <f t="shared" ref="D74:D77" si="14">D73+1</f>
+        <v>9</v>
+      </c>
+      <c r="E74" s="11">
+        <v>10</v>
+      </c>
+      <c r="F74" s="13">
+        <v>0</v>
+      </c>
+      <c r="G74" s="13"/>
+    </row>
+    <row r="75" spans="1:7" ht="17.399999999999999">
+      <c r="A75" s="19"/>
+      <c r="B75" s="11">
+        <f t="shared" si="13"/>
+        <v>53</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="11">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="E75" s="11">
+        <v>10</v>
+      </c>
+      <c r="F75" s="13">
+        <v>0</v>
+      </c>
+      <c r="G75" s="13"/>
+    </row>
+    <row r="76" spans="1:7" ht="17.399999999999999">
+      <c r="A76" s="19"/>
+      <c r="B76" s="11">
+        <f t="shared" si="13"/>
+        <v>54</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="11">
+        <f t="shared" si="14"/>
+        <v>11</v>
+      </c>
+      <c r="E76" s="11">
+        <v>10</v>
+      </c>
+      <c r="F76" s="13">
+        <v>2</v>
+      </c>
+      <c r="G76" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="17.399999999999999">
+      <c r="A77" s="19"/>
+      <c r="B77" s="11">
+        <f t="shared" si="13"/>
+        <v>55</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="11">
+        <f t="shared" si="14"/>
+        <v>12</v>
+      </c>
+      <c r="E77" s="11">
+        <v>10</v>
+      </c>
+      <c r="F77" s="13">
+        <v>1</v>
+      </c>
+      <c r="G77" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A78" s="19"/>
+      <c r="B78" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" s="25"/>
+      <c r="D78" s="25"/>
+      <c r="E78" s="26"/>
+      <c r="F78" s="1">
+        <f>SUM(F71:F77)</f>
+        <v>18.75</v>
+      </c>
+      <c r="G78" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="23">
+    <mergeCell ref="A69:A78"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="A59:A68"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="A49:A58"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B58:E58"/>
     <mergeCell ref="A1:A9"/>
     <mergeCell ref="A10:A19"/>
     <mergeCell ref="A39:A48"/>
@@ -2330,12 +2551,6 @@
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A59:A68"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="A49:A58"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B58:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>